<commit_message>
--Add 1426 1. 飞行近战。
</commit_message>
<xml_diff>
--- a/Assets/Tables/table_enemy.xlsx
+++ b/Assets/Tables/table_enemy.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="461">
   <si>
     <t>id</t>
   </si>
@@ -1061,6 +1061,21 @@
   </si>
   <si>
     <t>CHARGE_SPEED=30;MAX_CHARGE_SEC=4;FLYAROUND_DEG=80,160;FLYAROUND_RADIUS=8,16;FLYAROUND_COUNT_MAX=6;FLYAROUND_COUNT_MIN=4;ATTACK_DIS=2</t>
+  </si>
+  <si>
+    <t>enemy_201706</t>
+  </si>
+  <si>
+    <t>飞行近战</t>
+  </si>
+  <si>
+    <t>sharp=3</t>
+  </si>
+  <si>
+    <t>BT_Common_FlyMelee</t>
+  </si>
+  <si>
+    <t>FLYAROUND_DEG_1=60,120;FLYAROUND_RADIUS_1=5,6;FLYAROUND_COUNT_MAX_1=1;FLYAROUND_COUNT_MIN_1=1;FLYAROUND_DEG_2=0,180;FLYAROUND_RADIUS_2=1,2;FLYAROUND_COUNT_MAX_2=1;FLYAROUND_COUNT_MIN_2=1;BEFORE_ATTACK_SEC=0.2;AFTER_ATTACK_SEC=0.3;BEGIN_ATK_DIS=1;ATK_DIS=1.5;ATK_CD=1</t>
   </si>
   <si>
     <t>parm_key</t>
@@ -3472,11 +3487,11 @@
   <dimension ref="A1:AT86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="AM58" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J88" sqref="J88"/>
+      <selection pane="bottomRight" activeCell="AT84" sqref="AT84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
@@ -10798,9 +10813,7 @@
       <c r="B82" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="C82" s="25" t="s">
-        <v>180</v>
-      </c>
+      <c r="C82" s="25"/>
       <c r="D82" s="25" t="s">
         <v>236</v>
       </c>
@@ -10891,9 +10904,7 @@
       <c r="B83" s="24" t="s">
         <v>241</v>
       </c>
-      <c r="C83" s="25" t="s">
-        <v>151</v>
-      </c>
+      <c r="C83" s="25"/>
       <c r="D83" s="25" t="s">
         <v>242</v>
       </c>
@@ -10980,6 +10991,82 @@
       <c r="AS83" s="51"/>
       <c r="AT83" s="81" t="s">
         <v>245</v>
+      </c>
+    </row>
+    <row r="84" spans="1:46">
+      <c r="A84" s="24">
+        <v>209102</v>
+      </c>
+      <c r="B84" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="C84" s="25"/>
+      <c r="D84" s="25" t="s">
+        <v>247</v>
+      </c>
+      <c r="G84" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H84" s="24">
+        <v>3000</v>
+      </c>
+      <c r="I84" s="24">
+        <v>0</v>
+      </c>
+      <c r="J84" s="24">
+        <v>500</v>
+      </c>
+      <c r="M84" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="N84" s="47">
+        <v>3</v>
+      </c>
+      <c r="V84" s="24">
+        <v>4</v>
+      </c>
+      <c r="W84" s="48">
+        <v>8</v>
+      </c>
+      <c r="X84" s="49">
+        <v>4000</v>
+      </c>
+      <c r="AA84" s="69" t="s">
+        <v>238</v>
+      </c>
+      <c r="AB84" s="50" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC84" s="69" t="s">
+        <v>249</v>
+      </c>
+      <c r="AE84" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="AF84" s="24"/>
+      <c r="AG84" t="s">
+        <v>228</v>
+      </c>
+      <c r="AH84" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI84" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ84" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK84" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN84" s="24">
+        <v>0</v>
+      </c>
+      <c r="AO84" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="AT84" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="86" spans="1:46">
@@ -11046,19 +11133,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>0</v>
@@ -11067,19 +11154,19 @@
         <v>1</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="Q3" s="5" t="s">
         <v>0</v>
@@ -11088,19 +11175,19 @@
         <v>1</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="Y3" s="5" t="s">
         <v>0</v>
@@ -11109,19 +11196,19 @@
         <v>1</v>
       </c>
       <c r="AA3" s="5" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="AB3" s="5" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="AC3" s="5" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="AD3" s="5" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="AE3" s="5" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:42">
@@ -11140,10 +11227,10 @@
         <v>毒刺果实丛</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="M4" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11163,7 +11250,7 @@
         <v>涂涂鸟</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="U4" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11183,7 +11270,7 @@
         <v>金鱼</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="AC4" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11212,7 +11299,7 @@
         <v>毒刺果实丛</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="M5" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11232,7 +11319,7 @@
         <v>涂涂鸟</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="U5" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11252,10 +11339,10 @@
         <v>金鱼</v>
       </c>
       <c r="AA5" s="3" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="AB5" s="5" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="AC5" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11284,7 +11371,7 @@
         <v>毒刺果实丛</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="M6" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11304,7 +11391,7 @@
         <v>涂涂鸟</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="U6" s="92" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11324,7 +11411,7 @@
         <v>金鱼</v>
       </c>
       <c r="AA6" s="3" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="AC6" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11337,16 +11424,16 @@
         <v>237</v>
       </c>
       <c r="AF6" s="29" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="AG6" s="29" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="AH6" s="29" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="AI6" s="29" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:42">
@@ -11365,7 +11452,7 @@
         <v>画中仙</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="M7" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11385,7 +11472,7 @@
         <v>涂涂鸟</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="U7" s="5" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11405,7 +11492,7 @@
         <v>金鱼</v>
       </c>
       <c r="AA7" s="3" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="AC7" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11467,7 +11554,7 @@
         <v>画中仙</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="M8" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11487,7 +11574,7 @@
         <v>涂涂鸟</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="U8" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11507,10 +11594,10 @@
         <v>金鱼</v>
       </c>
       <c r="AA8" s="3" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="AB8" s="5" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="AC8" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11526,7 +11613,7 @@
         <v>201402</v>
       </c>
       <c r="AG8" s="40" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="AH8" s="3">
         <f t="shared" ref="AH8:AH25" si="0">IFERROR(COLUMNS(_xlfn.TEXTSPLIT(AG8,";")),0)</f>
@@ -11573,7 +11660,7 @@
         <v>画中仙</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="M9" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11593,7 +11680,7 @@
         <v>涂涂鸟</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="U9" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11613,7 +11700,7 @@
         <v>金鱼</v>
       </c>
       <c r="AA9" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AC9" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11674,7 +11761,7 @@
         <v>画中仙</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="M10" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11694,7 +11781,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="U10" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11714,7 +11801,7 @@
         <v>金鱼</v>
       </c>
       <c r="AA10" s="3" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="AC10" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11730,7 +11817,7 @@
         <v>201404</v>
       </c>
       <c r="AG10" s="40" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="AH10" s="3">
         <f t="shared" si="0"/>
@@ -11777,7 +11864,7 @@
         <v>画中仙</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="M11" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11797,7 +11884,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="U11" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11817,10 +11904,10 @@
         <v>金鱼</v>
       </c>
       <c r="AA11" s="3" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="AB11" s="5" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="AC11" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11836,7 +11923,7 @@
         <v>201405</v>
       </c>
       <c r="AG11" s="40" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="AH11" s="3">
         <f t="shared" si="0"/>
@@ -11883,7 +11970,7 @@
         <v>画中仙</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="M12" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11903,7 +11990,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S12" s="3" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="U12" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11923,10 +12010,10 @@
         <v>金鱼</v>
       </c>
       <c r="AA12" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="AB12" s="5" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="AC12" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11942,7 +12029,7 @@
         <v>201406</v>
       </c>
       <c r="AG12" s="40" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="AH12" s="3">
         <f t="shared" si="0"/>
@@ -11982,7 +12069,7 @@
         <v>画中仙</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="M13" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12002,7 +12089,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S13" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="U13" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12022,7 +12109,7 @@
         <v>金鱼泡泡</v>
       </c>
       <c r="AA13" s="3" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="AC13" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12038,7 +12125,7 @@
         <v>201407</v>
       </c>
       <c r="AG13" s="40" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="AH13" s="3">
         <f t="shared" si="0"/>
@@ -12078,7 +12165,7 @@
         <v>画中仙</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="M14" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12098,7 +12185,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S14" s="3" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="U14" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12118,7 +12205,7 @@
         <v>金鱼泡泡</v>
       </c>
       <c r="AA14" s="3" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="AC14" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12172,7 +12259,7 @@
         <v>鱼妖</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="M15" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12192,7 +12279,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="U15" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12212,7 +12299,7 @@
         <v>海藻小妖</v>
       </c>
       <c r="AA15" s="3" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="AC15" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12266,7 +12353,7 @@
         <v>鱼妖</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="M16" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12286,7 +12373,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="U16" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12306,10 +12393,10 @@
         <v>海藻小妖</v>
       </c>
       <c r="AA16" s="3" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="AB16" s="5" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="AC16" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12363,10 +12450,10 @@
         <v>鬼瓮</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="M17" s="5" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12386,7 +12473,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="U17" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12406,7 +12493,7 @@
         <v>海藻小妖</v>
       </c>
       <c r="AA17" s="3" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="AC17" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12460,7 +12547,7 @@
         <v>鬼狰</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="M18" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12480,7 +12567,7 @@
         <v>巨牙蝎</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="U18" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12500,7 +12587,7 @@
         <v>海藻小妖</v>
       </c>
       <c r="AA18" s="3" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="AC18" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12554,7 +12641,7 @@
         <v>鬼狰</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="M19" s="5" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12574,7 +12661,7 @@
         <v>巨牙蝎</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="U19" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12594,10 +12681,10 @@
         <v>海藻小妖</v>
       </c>
       <c r="AA19" s="3" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="AB19" s="5" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="AC19" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12651,7 +12738,7 @@
         <v>鬼狰</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="M20" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12671,7 +12758,7 @@
         <v>巨牙蝎</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="U20" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12691,7 +12778,7 @@
         <v>海藻小妖</v>
       </c>
       <c r="AA20" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AC20" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12746,10 +12833,10 @@
         <v>巨牙蝎</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="T21" s="5" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="U21" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12769,7 +12856,7 @@
         <v>海藻小妖</v>
       </c>
       <c r="AA21" s="3" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="AC21" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12824,7 +12911,7 @@
         <v>巨牙蝎</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="U22" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12844,7 +12931,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA22" s="3" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="AC22" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12899,7 +12986,7 @@
         <v>巨牙蝎</v>
       </c>
       <c r="S23" s="3" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="U23" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12919,7 +13006,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA23" s="3" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="AC23" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12974,7 +13061,7 @@
         <v>巨牙蝎</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="U24" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12994,7 +13081,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA24" s="3" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="AC24" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13049,7 +13136,7 @@
         <v>巨型石头人</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="U25" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13069,7 +13156,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA25" s="3" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="AC25" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13124,7 +13211,7 @@
         <v>巨型石头人</v>
       </c>
       <c r="S26" s="3" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="U26" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13144,7 +13231,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA26" s="3" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="AC26" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13167,7 +13254,7 @@
         <v>巨型石头人</v>
       </c>
       <c r="S27" s="3" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="U27" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13187,7 +13274,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA27" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AC27" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13210,7 +13297,7 @@
         <v>巨型石头人</v>
       </c>
       <c r="S28" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="U28" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13230,7 +13317,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA28" s="3" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="AC28" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13253,7 +13340,7 @@
         <v>巨型石头人</v>
       </c>
       <c r="S29" s="3" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="U29" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13273,7 +13360,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA29" s="3" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="AC29" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13296,7 +13383,7 @@
         <v>小石头人</v>
       </c>
       <c r="S30" s="3" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="U30" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13316,7 +13403,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA30" s="3" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="AC30" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13339,7 +13426,7 @@
         <v>小石头人</v>
       </c>
       <c r="S31" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="U31" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13359,7 +13446,7 @@
         <v>似目草</v>
       </c>
       <c r="AA31" s="3" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="AC31" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13382,7 +13469,7 @@
         <v>小石头人</v>
       </c>
       <c r="S32" s="3" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="U32" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13402,7 +13489,7 @@
         <v>似目草</v>
       </c>
       <c r="AA32" s="3" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="AC32" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13425,7 +13512,7 @@
         <v>小石头人</v>
       </c>
       <c r="S33" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="U33" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13445,7 +13532,7 @@
         <v>似目草</v>
       </c>
       <c r="AA33" s="5" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="AC33" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13471,7 +13558,7 @@
         <v>小石头人</v>
       </c>
       <c r="S34" s="3" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="U34" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13491,7 +13578,7 @@
         <v>脑型大水母</v>
       </c>
       <c r="AA34" s="3" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="AC34" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13513,7 +13600,7 @@
         <v>小石头人</v>
       </c>
       <c r="S35" s="3" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="T35" s="5"/>
       <c r="U35" s="3" t="str">
@@ -13534,7 +13621,7 @@
         <v>脑型大水母</v>
       </c>
       <c r="AA35" s="3" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="AC35" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13556,7 +13643,7 @@
         <v>小石头人</v>
       </c>
       <c r="S36" s="3" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="U36" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13576,7 +13663,7 @@
         <v>脑型大水母</v>
       </c>
       <c r="AA36" s="3" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="AC36" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13598,10 +13685,10 @@
         <v>大盾守卫</v>
       </c>
       <c r="S37" s="3" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="T37" s="5" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="U37" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13621,7 +13708,7 @@
         <v>脑型大水母</v>
       </c>
       <c r="AA37" s="3" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="AC37" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13634,13 +13721,13 @@
         <v>237</v>
       </c>
       <c r="AF37" s="29" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="AG37" s="29" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="AH37" s="29" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
     </row>
     <row r="38" spans="10:35">
@@ -13652,10 +13739,10 @@
         <v>大盾守卫</v>
       </c>
       <c r="S38" s="3" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="T38" s="5" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="U38" s="5" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13675,7 +13762,7 @@
         <v>脑型大水母</v>
       </c>
       <c r="AA38" s="3" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="AC38" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13712,7 +13799,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S39" s="3" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="U39" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13732,10 +13819,10 @@
         <v>脑型大水母</v>
       </c>
       <c r="AA39" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="AB39" s="5" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="AC39" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13771,7 +13858,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S40" s="3" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="U40" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13791,7 +13878,7 @@
         <v>脑型大水母</v>
       </c>
       <c r="AA40" s="3" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="AC40" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13827,7 +13914,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S41" s="3" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="U41" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13847,7 +13934,7 @@
         <v>针刺小水母</v>
       </c>
       <c r="AA41" s="3" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="AC41" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13883,7 +13970,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S42" s="3" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="U42" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13903,7 +13990,7 @@
         <v>针刺小水母</v>
       </c>
       <c r="AA42" s="3" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="AC42" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13939,7 +14026,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S43" s="3" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="U43" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13959,7 +14046,7 @@
         <v>针刺小水母</v>
       </c>
       <c r="AA43" s="3" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="AC43" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13995,7 +14082,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S44" s="3" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="U44" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14015,7 +14102,7 @@
         <v>针刺小水母</v>
       </c>
       <c r="AA44" s="3" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="AC44" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14051,7 +14138,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S45" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="U45" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14071,7 +14158,7 @@
         <v>针刺小水母</v>
       </c>
       <c r="AA45" s="3" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="AC45" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14107,7 +14194,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S46" s="3" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="U46" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14127,7 +14214,7 @@
         <v>针刺小水母</v>
       </c>
       <c r="AA46" s="3" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="AC46" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14163,7 +14250,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S47" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="U47" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14183,7 +14270,7 @@
         <v>印花水母</v>
       </c>
       <c r="AA47" s="3" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="AC47" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14219,7 +14306,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S48" s="3" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="U48" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14239,7 +14326,7 @@
         <v>印花水母</v>
       </c>
       <c r="AA48" s="3" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="AC48" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14275,10 +14362,10 @@
         <v>大盾守卫</v>
       </c>
       <c r="S49" s="3" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="T49" s="5" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="U49" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14298,7 +14385,7 @@
         <v>印花水母</v>
       </c>
       <c r="AA49" s="3" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="AC49" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14334,10 +14421,10 @@
         <v>基础守卫</v>
       </c>
       <c r="S50" s="3" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="T50" s="5" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="U50" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14357,7 +14444,7 @@
         <v>印花水母</v>
       </c>
       <c r="AA50" s="3" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="AC50" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14393,10 +14480,10 @@
         <v>基础守卫</v>
       </c>
       <c r="S51" s="3" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="T51" s="5" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="U51" s="5" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14416,7 +14503,7 @@
         <v>印花水母</v>
       </c>
       <c r="AA51" s="3" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="AC51" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14452,7 +14539,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S52" s="3" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="U52" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14472,7 +14559,7 @@
         <v>印花水母</v>
       </c>
       <c r="AA52" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AC52" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14508,7 +14595,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S53" s="3" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="U53" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14528,7 +14615,7 @@
         <v>混沌沼泽怪</v>
       </c>
       <c r="AA53" s="3" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="AC53" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14564,10 +14651,10 @@
         <v>基础守卫</v>
       </c>
       <c r="S54" s="3" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="T54" s="5" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="U54" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14587,7 +14674,7 @@
         <v>混沌沼泽怪</v>
       </c>
       <c r="AA54" s="3" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="AC54" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14623,10 +14710,10 @@
         <v>基础守卫</v>
       </c>
       <c r="S55" s="3" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="T55" s="5" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="U55" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14646,7 +14733,7 @@
         <v>混沌沼泽怪</v>
       </c>
       <c r="AA55" s="3" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="AC55" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14676,7 +14763,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S56" s="3" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="U56" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14696,7 +14783,7 @@
         <v>混沌沼泽怪</v>
       </c>
       <c r="AA56" s="3" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="AC56" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14726,7 +14813,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S57" s="3" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="U57" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14746,7 +14833,7 @@
         <v>混沌沼泽怪</v>
       </c>
       <c r="AA57" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AC57" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14776,7 +14863,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S58" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="U58" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14796,7 +14883,7 @@
         <v>混沌沼泽怪</v>
       </c>
       <c r="AA58" s="3" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="AC58" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14826,7 +14913,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S59" s="3" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="U59" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14846,7 +14933,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA59" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AC59" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14876,7 +14963,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S60" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="U60" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14896,7 +14983,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA60" s="3" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="AC60" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14926,7 +15013,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S61" s="3" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="U61" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14946,7 +15033,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA61" s="3" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="AC61" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14976,10 +15063,10 @@
         <v>基础守卫</v>
       </c>
       <c r="S62" s="3" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="T62" s="5" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="U62" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14999,7 +15086,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA62" s="3" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="AC62" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15029,7 +15116,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S63" s="3" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="U63" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15049,7 +15136,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA63" s="3" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="AC63" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15079,7 +15166,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S64" s="3" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="U64" s="5" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15099,7 +15186,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA64" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="AC64" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15129,7 +15216,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S65" s="3" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="U65" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15149,7 +15236,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA65" s="3" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="AC65" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15179,7 +15266,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S66" s="3" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="U66" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15199,7 +15286,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA66" s="3" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="AC66" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15229,7 +15316,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S67" s="3" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="U67" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15249,7 +15336,7 @@
         <v/>
       </c>
       <c r="AA67" s="3" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="AC67" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15279,7 +15366,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S68" s="3" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="U68" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15299,10 +15386,10 @@
         <v/>
       </c>
       <c r="AA68" s="3" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="AB68" s="5" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="AC68" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15332,7 +15419,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S69" s="3" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="U69" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15352,10 +15439,10 @@
         <v/>
       </c>
       <c r="AA69" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="AB69" s="5" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="AC69" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15385,7 +15472,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S70" s="3" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="U70" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15405,7 +15492,7 @@
         <v/>
       </c>
       <c r="AA70" s="3" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="AC70" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15435,7 +15522,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S71" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="U71" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15455,7 +15542,7 @@
         <v>贝壳乌贼</v>
       </c>
       <c r="AA71" s="3" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="AC71" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15485,7 +15572,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S72" s="3" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="U72" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15505,7 +15592,7 @@
         <v>贝壳乌贼</v>
       </c>
       <c r="AA72" s="3" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="AC72" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15535,7 +15622,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S73" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="U73" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15555,7 +15642,7 @@
         <v>贝壳乌贼</v>
       </c>
       <c r="AA73" s="3" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="AC73" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15585,7 +15672,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S74" s="3" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="U74" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15605,7 +15692,7 @@
         <v>贝壳乌贼</v>
       </c>
       <c r="AA74" s="3" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="AC74" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15635,10 +15722,10 @@
         <v>双刀守卫</v>
       </c>
       <c r="S75" s="3" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="T75" s="5" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="U75" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15658,7 +15745,7 @@
         <v>贝壳乌贼</v>
       </c>
       <c r="AA75" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AC75" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15688,7 +15775,7 @@
         <v>大仙人掌</v>
       </c>
       <c r="S76" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="U76" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15708,7 +15795,7 @@
         <v>贝壳乌贼</v>
       </c>
       <c r="AA76" s="3" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="AC76" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15738,7 +15825,7 @@
         <v>大仙人掌</v>
       </c>
       <c r="S77" s="3" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="U77" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15758,7 +15845,7 @@
         <v>弱小螃蟹</v>
       </c>
       <c r="AA77" s="3" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="AC77" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15788,10 +15875,10 @@
         <v>大仙人掌</v>
       </c>
       <c r="S78" s="3" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="T78" s="5" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="U78" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15811,7 +15898,7 @@
         <v>弱小螃蟹</v>
       </c>
       <c r="AA78" s="3" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="AC78" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15841,10 +15928,10 @@
         <v>大仙人掌</v>
       </c>
       <c r="S79" s="3" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="T79" s="5" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="U79" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15864,7 +15951,7 @@
         <v>弱小螃蟹</v>
       </c>
       <c r="AA79" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AC79" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15894,7 +15981,7 @@
         <v>小仙人掌</v>
       </c>
       <c r="S80" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="U80" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15914,7 +16001,7 @@
         <v>弱小螃蟹</v>
       </c>
       <c r="AA80" s="3" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="AC80" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15944,7 +16031,7 @@
         <v>小仙人掌</v>
       </c>
       <c r="S81" s="3" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="U81" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15964,7 +16051,7 @@
         <v>大钳螃蟹</v>
       </c>
       <c r="AA81" s="3" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="AC81" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15994,10 +16081,10 @@
         <v>小仙人掌</v>
       </c>
       <c r="S82" s="3" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="T82" s="5" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="U82" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16017,7 +16104,7 @@
         <v>大钳螃蟹</v>
       </c>
       <c r="AA82" s="3" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="AC82" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16047,10 +16134,10 @@
         <v>小仙人掌</v>
       </c>
       <c r="S83" s="3" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="T83" s="5" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="U83" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16070,7 +16157,7 @@
         <v>大钳螃蟹</v>
       </c>
       <c r="AA83" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AC83" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16100,7 +16187,7 @@
         <v>大风滚草</v>
       </c>
       <c r="S84" s="3" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="U84" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16120,7 +16207,7 @@
         <v>大钳螃蟹</v>
       </c>
       <c r="AA84" s="3" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="AC84" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16150,7 +16237,7 @@
         <v>大风滚草</v>
       </c>
       <c r="S85" s="3" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="U85" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16170,7 +16257,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA85" s="3" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="AC85" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16200,7 +16287,7 @@
         <v>大风滚草</v>
       </c>
       <c r="S86" s="3" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="U86" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16220,7 +16307,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA86" s="3" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="AC86" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16250,7 +16337,7 @@
         <v>大风滚草</v>
       </c>
       <c r="S87" s="3" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="U87" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16270,7 +16357,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA87" s="3" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="AC87" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16300,7 +16387,7 @@
         <v>大风滚草</v>
       </c>
       <c r="S88" s="3" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="U88" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16320,7 +16407,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA88" s="3" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="AC88" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16350,7 +16437,7 @@
         <v>小风滚草</v>
       </c>
       <c r="S89" s="3" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="U89" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16370,7 +16457,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA89" s="3" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="AC89" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16400,7 +16487,7 @@
         <v>小风滚草</v>
       </c>
       <c r="S90" s="3" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="U90" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16420,7 +16507,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA90" s="3" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="AC90" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16450,7 +16537,7 @@
         <v>小风滚草</v>
       </c>
       <c r="S91" s="3" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="U91" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16470,7 +16557,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA91" s="3" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="AC91" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16500,7 +16587,7 @@
         <v>小风滚草</v>
       </c>
       <c r="S92" s="3" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="U92" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16520,7 +16607,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA92" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="AC92" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16550,7 +16637,7 @@
         <v>小风滚草</v>
       </c>
       <c r="S93" s="3" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="U93" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16570,7 +16657,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA93" s="3" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="AC93" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16600,7 +16687,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA94" s="3" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="AC94" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16630,7 +16717,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA95" s="3" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="AC95" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16660,7 +16747,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA96" s="3" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="AC96" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16690,7 +16777,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA97" s="3" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="AC97" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16720,7 +16807,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA98" s="3" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="AC98" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16750,7 +16837,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA99" s="3" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="AC99" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16780,7 +16867,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA100" s="3" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="AC100" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16810,7 +16897,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA101" s="3" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="AC101" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16840,7 +16927,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA102" s="3" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="AC102" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16870,7 +16957,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA103" s="3" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="AC103" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16900,7 +16987,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA104" s="3" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="AC104" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16930,7 +17017,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA105" s="3" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="AC105" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16960,7 +17047,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA106" s="3" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="AC106" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16990,7 +17077,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA107" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AC107" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17020,7 +17107,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA108" s="3" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="AC108" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17050,7 +17137,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA109" s="3" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="AC109" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17080,7 +17167,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA110" s="3" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="AC110" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17110,7 +17197,7 @@
         <v>聒噪海贝</v>
       </c>
       <c r="AA111" s="3" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="AC111" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17140,10 +17227,10 @@
         <v>聒噪海贝</v>
       </c>
       <c r="AA112" s="3" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="AB112" s="5" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="AC112" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17173,10 +17260,10 @@
         <v>聒噪海贝</v>
       </c>
       <c r="AA113" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="AB113" s="5" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="AC113" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17206,7 +17293,7 @@
         <v>聒噪海贝</v>
       </c>
       <c r="AA114" s="3" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="AC114" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17236,7 +17323,7 @@
         <v>凶猛海贝</v>
       </c>
       <c r="AA115" s="3" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="AC115" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17266,10 +17353,10 @@
         <v>凶猛海贝</v>
       </c>
       <c r="AA116" s="3" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="AB116" s="5" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="AC116" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17299,10 +17386,10 @@
         <v>凶猛海贝</v>
       </c>
       <c r="AA117" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="AB117" s="5" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="AC117" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17332,7 +17419,7 @@
         <v>凶猛海贝</v>
       </c>
       <c r="AA118" s="3" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="AC118" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17362,7 +17449,7 @@
         <v>小·印花水母</v>
       </c>
       <c r="AA119" s="41" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="AC119" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17392,7 +17479,7 @@
         <v>小·印花水母</v>
       </c>
       <c r="AA120" s="41" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="AC120" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17422,7 +17509,7 @@
         <v>小·印花水母</v>
       </c>
       <c r="AA121" s="41" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="AC121" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17452,7 +17539,7 @@
         <v>小·印花水母</v>
       </c>
       <c r="AA122" s="41" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="AC122" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17482,7 +17569,7 @@
         <v>小·印花水母</v>
       </c>
       <c r="AA123" s="41" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="AC123" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17512,7 +17599,7 @@
         <v>小·印花水母</v>
       </c>
       <c r="AA124" s="41" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AC124" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17542,7 +17629,7 @@
         <v>小·聒噪海贝</v>
       </c>
       <c r="AA125" s="41" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="AC125" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17572,10 +17659,10 @@
         <v>小·聒噪海贝</v>
       </c>
       <c r="AA126" s="41" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="AB126" s="5" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="AC126" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17605,10 +17692,10 @@
         <v>小·聒噪海贝</v>
       </c>
       <c r="AA127" s="41" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="AB127" s="5" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="AC127" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17638,7 +17725,7 @@
         <v>小·聒噪海贝</v>
       </c>
       <c r="AA128" s="41" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="AC128" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17660,7 +17747,7 @@
         <v>小·海藻小妖</v>
       </c>
       <c r="AA129" s="41" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="AC129" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17682,10 +17769,10 @@
         <v>小·海藻小妖</v>
       </c>
       <c r="AA130" s="41" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="AB130" s="5" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="AC130" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17707,7 +17794,7 @@
         <v>小·海藻小妖</v>
       </c>
       <c r="AA131" s="41" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="AC131" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17729,7 +17816,7 @@
         <v>小·海藻小妖</v>
       </c>
       <c r="AA132" s="41" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="AC132" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17751,10 +17838,10 @@
         <v>小·海藻小妖</v>
       </c>
       <c r="AA133" s="41" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="AB133" s="5" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="AC133" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17776,7 +17863,7 @@
         <v>小·海藻小妖</v>
       </c>
       <c r="AA134" s="41" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AC134" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17798,7 +17885,7 @@
         <v>小·海藻小妖</v>
       </c>
       <c r="AA135" s="41" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="AC135" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17859,58 +17946,58 @@
   <sheetData>
     <row r="1" ht="28.5" spans="1:30">
       <c r="A1" s="29" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="H1" s="29" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="I1" s="29" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="J1" s="29" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="K1" s="29" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="L1" s="29" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="M1" s="32" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="N1" s="32" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="O1" s="32" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="P1" s="32" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="Q1" s="32" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="R1" s="32" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="T1" s="33" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
       <c r="V1" s="33" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
     </row>
     <row r="2" spans="1:30">
@@ -18123,14 +18210,14 @@
         <v/>
       </c>
       <c r="Z7" s="35" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="AA7" s="35"/>
       <c r="AB7" s="36">
         <v>10000</v>
       </c>
       <c r="AC7" s="37" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="AD7" s="37"/>
     </row>
@@ -18175,7 +18262,7 @@
         <v>10000=0.0048;600109=0.0001</v>
       </c>
       <c r="Z8" s="35" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="AA8" s="35"/>
       <c r="AB8" s="38">
@@ -18183,7 +18270,7 @@
         <v>0.0001</v>
       </c>
       <c r="AC8" s="37" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
       <c r="AD8" s="37"/>
     </row>
@@ -18228,14 +18315,14 @@
         <v>10000=0.0048;600109=0.0001</v>
       </c>
       <c r="Z9" s="35" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="AA9" s="35"/>
       <c r="AB9" s="36">
         <v>300</v>
       </c>
       <c r="AC9" s="37" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
       <c r="AD9" s="37"/>
     </row>
@@ -20788,7 +20875,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{f872b41b-7706-485b-92bc-d31c426e93d6}</x14:id>
+          <x14:id>{a53faaef-6bee-441c-a0d3-4a3c263dbab7}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -20801,7 +20888,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{f872b41b-7706-485b-92bc-d31c426e93d6}">
+          <x14:cfRule type="dataBar" id="{a53faaef-6bee-441c-a0d3-4a3c263dbab7}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>-10</xm:f>
@@ -20855,17 +20942,17 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="D1" s="14"/>
       <c r="E1" s="6" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
@@ -20875,15 +20962,15 @@
       <c r="L1" s="15"/>
       <c r="M1" s="16"/>
       <c r="N1" s="6" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="P1" s="16"/>
       <c r="Q1" s="16"/>
       <c r="R1" s="6" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2" s="7" customFormat="1" spans="1:18">
@@ -20898,7 +20985,7 @@
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="7" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>32</v>
@@ -20914,7 +21001,7 @@
         <v>28</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="P2" s="16"/>
       <c r="Q2" s="16"/>
@@ -20924,58 +21011,58 @@
     </row>
     <row r="3" s="8" customFormat="1" ht="52.5" spans="1:18">
       <c r="A3" s="18" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
       <c r="K3" s="21" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
       <c r="L3" s="21" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="M3" s="22" t="s">
         <v>61</v>
       </c>
       <c r="N3" s="20" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="O3" s="20" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="P3" s="22" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="Q3" s="22" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -21005,7 +21092,7 @@
         <v>1311101</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="N4" s="23" t="str">
         <f>_xlfn.TEXTJOIN("_",1,"Car_AI",$M4)</f>
@@ -21052,7 +21139,7 @@
         <v>1311101</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="N5" s="23" t="str">
         <f t="shared" ref="N5:N13" si="0">_xlfn.TEXTJOIN("_",1,"Car_AI",$M5)</f>
@@ -21099,7 +21186,7 @@
         <v>1311101</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="N6" s="23" t="str">
         <f t="shared" si="0"/>
@@ -21146,7 +21233,7 @@
         <v>1311101</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="N7" s="23" t="str">
         <f t="shared" si="0"/>
@@ -21196,7 +21283,7 @@
         <v>1311101</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="N8" s="23" t="str">
         <f t="shared" si="0"/>
@@ -21246,7 +21333,7 @@
         <v>1311101</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="N9" s="23" t="str">
         <f t="shared" si="0"/>
@@ -21293,7 +21380,7 @@
         <v>1321101</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="N11" s="23" t="str">
         <f t="shared" si="0"/>
@@ -21340,7 +21427,7 @@
         <v>1321101</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="N12" s="23" t="str">
         <f t="shared" si="0"/>
@@ -21387,7 +21474,7 @@
         <v>1321101</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="N13" s="23" t="str">
         <f t="shared" si="0"/>
@@ -21440,7 +21527,7 @@
         <v>1311101</v>
       </c>
       <c r="M15" s="11" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="N15" s="23" t="str">
         <f t="shared" ref="N15:N21" si="2">_xlfn.TEXTJOIN("_",1,"Car_AI",$M15)</f>
@@ -21490,7 +21577,7 @@
         <v>1311102</v>
       </c>
       <c r="M16" s="11" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="N16" s="23" t="str">
         <f t="shared" si="2"/>
@@ -21543,7 +21630,7 @@
         <v>1311101</v>
       </c>
       <c r="M18" s="11" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="N18" s="23" t="str">
         <f t="shared" si="2"/>
@@ -21596,7 +21683,7 @@
         <v>1311102</v>
       </c>
       <c r="M19" s="11" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="N19" s="23" t="str">
         <f t="shared" si="2"/>
@@ -21649,7 +21736,7 @@
         <v>1311101</v>
       </c>
       <c r="M20" s="11" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="N20" s="23" t="str">
         <f t="shared" si="2"/>
@@ -21702,7 +21789,7 @@
         <v>1311102</v>
       </c>
       <c r="M21" s="11" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="N21" s="23" t="str">
         <f t="shared" si="2"/>
@@ -21733,7 +21820,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="E23" s="3">
         <v>101101</v>
@@ -21749,10 +21836,10 @@
         <v>1321101</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="N23" s="23" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="O23" s="3" t="str">
         <f t="shared" si="1"/>
@@ -21795,7 +21882,7 @@
         <v>1321101</v>
       </c>
       <c r="M25" s="11" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="N25" s="23" t="str">
         <f t="shared" ref="N25:N29" si="3">_xlfn.TEXTJOIN("_",1,"Car_AI",$M25)</f>
@@ -21845,7 +21932,7 @@
         <v>1321101</v>
       </c>
       <c r="M26" s="11" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="N26" s="23" t="str">
         <f t="shared" si="3"/>
@@ -21892,7 +21979,7 @@
         <v>1321101</v>
       </c>
       <c r="M28" s="11" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="N28" s="23" t="str">
         <f t="shared" si="3"/>
@@ -21942,7 +22029,7 @@
         <v>1321101</v>
       </c>
       <c r="M29" s="11" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="N29" s="23" t="str">
         <f t="shared" si="3"/>
@@ -21987,7 +22074,7 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" s="4" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -21999,7 +22086,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
     </row>
     <row r="4" spans="2:4">
@@ -22007,7 +22094,7 @@
         <v>10000</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="D4" s="3"/>
     </row>
@@ -22021,7 +22108,7 @@
         <v>600101</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="D6" s="3"/>
     </row>
@@ -22030,7 +22117,7 @@
         <v>600102</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="D7" s="3"/>
     </row>
@@ -22039,7 +22126,7 @@
         <v>600103</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="D8" s="3"/>
     </row>
@@ -22048,7 +22135,7 @@
         <v>600104</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="D9" s="3"/>
     </row>
@@ -22057,7 +22144,7 @@
         <v>600105</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="D10" s="3"/>
     </row>
@@ -22066,7 +22153,7 @@
         <v>600106</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="D11" s="3"/>
     </row>
@@ -22075,7 +22162,7 @@
         <v>600107</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="D12" s="3"/>
     </row>
@@ -22084,7 +22171,7 @@
         <v>600108</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="D13" s="3"/>
     </row>
@@ -22093,7 +22180,7 @@
         <v>600109</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="D14" s="3"/>
     </row>
@@ -22102,7 +22189,7 @@
         <v>600110</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="D15" s="3"/>
     </row>
@@ -22116,7 +22203,7 @@
         <v>600401</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="D17" s="3"/>
     </row>
@@ -22125,7 +22212,7 @@
         <v>600402</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="D18" s="3"/>
     </row>
@@ -22134,7 +22221,7 @@
         <v>600403</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="D19" s="3"/>
     </row>
@@ -22143,7 +22230,7 @@
         <v>600404</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="D20" s="3"/>
     </row>
@@ -22152,7 +22239,7 @@
         <v>600405</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="D21" s="3"/>
     </row>
@@ -22161,7 +22248,7 @@
         <v>600406</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="D22" s="3"/>
     </row>
@@ -22170,7 +22257,7 @@
         <v>600407</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="D23" s="3"/>
     </row>
@@ -22179,7 +22266,7 @@
         <v>600408</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="D24" s="3"/>
     </row>
@@ -22188,7 +22275,7 @@
         <v>600409</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D25" s="3"/>
     </row>
@@ -22197,7 +22284,7 @@
         <v>600410</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="D26" s="3"/>
     </row>
@@ -22211,7 +22298,7 @@
         <v>600701</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="D28" s="3"/>
     </row>
@@ -22220,7 +22307,7 @@
         <v>600702</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="D29" s="3"/>
     </row>
@@ -22229,7 +22316,7 @@
         <v>600703</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="D30" s="3"/>
     </row>
@@ -22238,7 +22325,7 @@
         <v>600704</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="D31" s="3"/>
     </row>
@@ -22247,7 +22334,7 @@
         <v>600705</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="D32" s="3"/>
     </row>
@@ -22256,7 +22343,7 @@
         <v>600706</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="D33" s="3"/>
     </row>
@@ -22265,7 +22352,7 @@
         <v>600707</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="D34" s="3"/>
     </row>
@@ -22274,7 +22361,7 @@
         <v>600708</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c r="D35" s="3"/>
     </row>
@@ -22283,7 +22370,7 @@
         <v>600709</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c r="D36" s="3"/>
     </row>
@@ -22292,7 +22379,7 @@
         <v>600710</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c r="D37" s="3"/>
     </row>
@@ -22306,7 +22393,7 @@
         <v>600801</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="D39" s="3">
         <v>5</v>
@@ -22317,7 +22404,7 @@
         <v>600802</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
       <c r="D40" s="3">
         <v>55</v>
@@ -22328,7 +22415,7 @@
         <v>600803</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>428</v>
+        <v>433</v>
       </c>
       <c r="D41" s="3">
         <v>20</v>
@@ -22339,7 +22426,7 @@
         <v>600804</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="D42" s="3">
         <v>45</v>
@@ -22350,7 +22437,7 @@
         <v>600805</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="D43" s="3">
         <v>30</v>
@@ -22361,7 +22448,7 @@
         <v>600806</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
       <c r="D44" s="3">
         <v>3</v>
@@ -22372,7 +22459,7 @@
         <v>600807</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="D45" s="3">
         <v>15</v>
@@ -22383,7 +22470,7 @@
         <v>600808</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="D46" s="3">
         <v>2</v>
@@ -22394,7 +22481,7 @@
         <v>600809</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="D47" s="3">
         <v>15</v>
@@ -22405,7 +22492,7 @@
         <v>600810</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
       <c r="D48" s="3">
         <v>35</v>
@@ -22416,7 +22503,7 @@
         <v>600811</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="D49" s="3">
         <v>20</v>
@@ -22427,7 +22514,7 @@
         <v>600812</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="D50" s="3">
         <v>20</v>
@@ -22438,7 +22525,7 @@
         <v>600813</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="D51" s="3">
         <v>6</v>
@@ -22483,73 +22570,73 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>446</v>
+        <v>451</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="C7" s="2" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="C8" s="2" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="C9" s="2" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
     </row>
     <row r="11" spans="1:13">

</xml_diff>

<commit_message>
--Add 1608 1. 跳跃近战。
</commit_message>
<xml_diff>
--- a/Assets/Tables/table_enemy.xlsx
+++ b/Assets/Tables/table_enemy.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1391" uniqueCount="461">
   <si>
     <t>id</t>
   </si>
@@ -1030,9 +1030,6 @@
     <t>FLYAROUND_DEG=10,170;FLYAROUND_RADIUS=5,12</t>
   </si>
   <si>
-    <t>enemy_201870</t>
-  </si>
-  <si>
     <t>飞行远程</t>
   </si>
   <si>
@@ -1048,9 +1045,6 @@
     <t>FLYAROUND_DEG=30,150;FLYAROUND_RADIUS=8,12;FLYAROUND_COUNT_MAX=1;FLYAROUND_COUNT_MIN=1;BEFORE_ATTACK_SEC=0.6;AFTER_ATTACK_SEC=0.4;RUNNING_FIRE_COUNT=3</t>
   </si>
   <si>
-    <t>enemy_201701</t>
-  </si>
-  <si>
     <t>飞行冲刺</t>
   </si>
   <si>
@@ -1063,9 +1057,6 @@
     <t>CHARGE_SPEED=30;MAX_CHARGE_SEC=4;FLYAROUND_DEG=80,160;FLYAROUND_RADIUS=8,16;FLYAROUND_COUNT_MAX=6;FLYAROUND_COUNT_MIN=4;ATTACK_DIS=2</t>
   </si>
   <si>
-    <t>enemy_201706</t>
-  </si>
-  <si>
     <t>飞行近战</t>
   </si>
   <si>
@@ -1076,6 +1067,15 @@
   </si>
   <si>
     <t>FLYAROUND_DEG_1=60,120;FLYAROUND_RADIUS_1=5,6;FLYAROUND_COUNT_MAX_1=1;FLYAROUND_COUNT_MIN_1=1;FLYAROUND_DEG_2=0,180;FLYAROUND_RADIUS_2=1,2;FLYAROUND_COUNT_MAX_2=1;FLYAROUND_COUNT_MIN_2=1;BEFORE_ATTACK_SEC=0.2;AFTER_ATTACK_SEC=0.3;BEGIN_ATK_DIS=1;ATK_DIS=1.5;ATK_CD=1</t>
+  </si>
+  <si>
+    <t>跳跃近战</t>
+  </si>
+  <si>
+    <t>BT_Common_JumpMelee</t>
+  </si>
+  <si>
+    <t>JUMP_CD=0.58;ATK_AREA=1,2;JUMP_VELOCITY_X_MAX=20;JUMP_HEIGHT_AREA=1,2</t>
   </si>
   <si>
     <t>parm_key</t>
@@ -3487,11 +3487,11 @@
   <dimension ref="A1:AT86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="AM58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="AM61" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AT84" sqref="AT84"/>
+      <selection pane="bottomRight" activeCell="AT85" sqref="AT85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
@@ -10810,12 +10810,9 @@
       <c r="A82" s="24">
         <v>209100</v>
       </c>
-      <c r="B82" s="24" t="s">
+      <c r="B82" s="24"/>
+      <c r="D82" s="25" t="s">
         <v>235</v>
-      </c>
-      <c r="C82" s="25"/>
-      <c r="D82" s="25" t="s">
-        <v>236</v>
       </c>
       <c r="E82" s="66"/>
       <c r="F82" s="66"/>
@@ -10832,7 +10829,7 @@
         <v>1000</v>
       </c>
       <c r="M82" s="24" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N82" s="68"/>
       <c r="O82" s="68"/>
@@ -10852,13 +10849,11 @@
       <c r="Y82" s="80"/>
       <c r="Z82" s="80"/>
       <c r="AA82" s="69" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB82" s="50"/>
+      <c r="AC82" s="69" t="s">
         <v>238</v>
-      </c>
-      <c r="AB82" s="50" t="s">
-        <v>224</v>
-      </c>
-      <c r="AC82" s="69" t="s">
-        <v>239</v>
       </c>
       <c r="AD82" s="67">
         <v>201870</v>
@@ -10867,7 +10862,7 @@
         <v>0.15</v>
       </c>
       <c r="AF82" s="67" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG82" s="69" t="s">
         <v>228</v>
@@ -10891,22 +10886,20 @@
         <v>0</v>
       </c>
       <c r="AO82" s="67" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AT82" s="81" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="83" customFormat="1" spans="1:46">
       <c r="A83" s="24">
         <v>209101</v>
       </c>
-      <c r="B83" s="24" t="s">
-        <v>241</v>
-      </c>
+      <c r="B83" s="24"/>
       <c r="C83" s="25"/>
       <c r="D83" s="25" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E83" s="66"/>
       <c r="F83" s="66"/>
@@ -10925,7 +10918,7 @@
       <c r="K83" s="24"/>
       <c r="L83" s="24"/>
       <c r="M83" s="24" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="N83" s="68">
         <v>4</v>
@@ -10949,13 +10942,11 @@
       <c r="Y83" s="80"/>
       <c r="Z83" s="80"/>
       <c r="AA83" s="69" t="s">
-        <v>238</v>
-      </c>
-      <c r="AB83" s="50" t="s">
-        <v>224</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="AB83" s="50"/>
       <c r="AC83" s="69" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="AD83" s="67"/>
       <c r="AE83" s="24">
@@ -10983,26 +10974,23 @@
         <v>0</v>
       </c>
       <c r="AO83" s="67" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AP83" s="51"/>
       <c r="AQ83" s="51"/>
       <c r="AR83" s="51"/>
       <c r="AS83" s="51"/>
       <c r="AT83" s="81" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="84" spans="1:46">
       <c r="A84" s="24">
         <v>209102</v>
       </c>
-      <c r="B84" s="24" t="s">
-        <v>246</v>
-      </c>
-      <c r="C84" s="25"/>
+      <c r="B84" s="24"/>
       <c r="D84" s="25" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G84" s="24" t="s">
         <v>77</v>
@@ -11017,7 +11005,7 @@
         <v>500</v>
       </c>
       <c r="M84" s="24" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="N84" s="47">
         <v>3</v>
@@ -11032,18 +11020,15 @@
         <v>4000</v>
       </c>
       <c r="AA84" s="69" t="s">
-        <v>238</v>
-      </c>
-      <c r="AB84" s="50" t="s">
-        <v>224</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="AB84" s="50"/>
       <c r="AC84" s="69" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="AE84" s="24">
         <v>0.5</v>
       </c>
-      <c r="AF84" s="24"/>
       <c r="AG84" t="s">
         <v>228</v>
       </c>
@@ -11063,9 +11048,76 @@
         <v>0</v>
       </c>
       <c r="AO84" s="24" t="s">
+        <v>236</v>
+      </c>
+      <c r="AT84" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="85" spans="1:46">
+      <c r="A85" s="24">
+        <v>209103</v>
+      </c>
+      <c r="B85" s="24"/>
+      <c r="C85" s="25"/>
+      <c r="D85" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="G85" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H85" s="24">
+        <v>3000</v>
+      </c>
+      <c r="I85" s="24">
+        <v>0</v>
+      </c>
+      <c r="J85" s="24">
+        <v>7.12</v>
+      </c>
+      <c r="K85" s="24"/>
+      <c r="M85" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="N85" s="47">
+        <v>3</v>
+      </c>
+      <c r="AA85" s="69" t="s">
         <v>237</v>
       </c>
-      <c r="AT84" t="s">
+      <c r="AB85" s="50"/>
+      <c r="AC85" s="69" t="s">
+        <v>249</v>
+      </c>
+      <c r="AE85" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="AF85" s="24"/>
+      <c r="AG85" t="s">
+        <v>228</v>
+      </c>
+      <c r="AH85" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI85" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ85" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK85" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM85" s="51" t="s">
+        <v>183</v>
+      </c>
+      <c r="AN85" s="24">
+        <v>0</v>
+      </c>
+      <c r="AO85" s="24" t="s">
+        <v>236</v>
+      </c>
+      <c r="AT85" t="s">
         <v>250</v>
       </c>
     </row>
@@ -11240,7 +11292,7 @@
         <v>4</v>
       </c>
       <c r="O4" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Q4" s="3">
         <v>201701</v>
@@ -11260,7 +11312,7 @@
         <v>30</v>
       </c>
       <c r="W4" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y4" s="3">
         <v>201801</v>
@@ -11329,7 +11381,7 @@
         <v>4</v>
       </c>
       <c r="W5" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y5" s="3">
         <v>201801</v>
@@ -11421,7 +11473,7 @@
         <v>6</v>
       </c>
       <c r="AE6" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF6" s="29" t="s">
         <v>266</v>
@@ -11502,7 +11554,7 @@
         <v>4</v>
       </c>
       <c r="AE7" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF7" s="3">
         <v>201401</v>
@@ -11584,7 +11636,7 @@
         <v>6</v>
       </c>
       <c r="W8" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y8" s="3">
         <v>201801</v>
@@ -11670,7 +11722,7 @@
         <v>6</v>
       </c>
       <c r="O9" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Q9" s="3">
         <v>201701</v>
@@ -11690,7 +11742,7 @@
         <v>4</v>
       </c>
       <c r="W9" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y9" s="3">
         <v>201801</v>
@@ -11710,7 +11762,7 @@
         <v>0.2</v>
       </c>
       <c r="AE9" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF9" s="3">
         <v>201403</v>
@@ -11771,7 +11823,7 @@
         <v>4</v>
       </c>
       <c r="O10" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Q10" s="3">
         <v>201702</v>
@@ -11791,7 +11843,7 @@
         <v>4</v>
       </c>
       <c r="W10" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y10" s="3">
         <v>201801</v>
@@ -11811,7 +11863,7 @@
         <v>0.5</v>
       </c>
       <c r="AE10" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF10" s="3">
         <v>201404</v>
@@ -11894,7 +11946,7 @@
         <v>3</v>
       </c>
       <c r="W11" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y11" s="3">
         <v>201801</v>
@@ -11917,7 +11969,7 @@
         <v>1</v>
       </c>
       <c r="AE11" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF11" s="3">
         <v>201405</v>
@@ -11980,7 +12032,7 @@
         <v>0.2</v>
       </c>
       <c r="O12" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Q12" s="3">
         <v>201702</v>
@@ -12000,7 +12052,7 @@
         <v>6</v>
       </c>
       <c r="W12" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y12" s="3">
         <v>201801</v>
@@ -12023,7 +12075,7 @@
         <v>0.3</v>
       </c>
       <c r="AE12" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF12" s="3">
         <v>201406</v>
@@ -12079,7 +12131,7 @@
         <v>3</v>
       </c>
       <c r="O13" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Q13" s="3">
         <v>201702</v>
@@ -12099,7 +12151,7 @@
         <v>0.2</v>
       </c>
       <c r="W13" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y13" s="3">
         <v>201802</v>
@@ -12119,7 +12171,7 @@
         <v>1.2</v>
       </c>
       <c r="AE13" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF13" s="3">
         <v>201407</v>
@@ -12195,7 +12247,7 @@
         <v>0.3</v>
       </c>
       <c r="W14" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y14" s="3">
         <v>201802</v>
@@ -12215,7 +12267,7 @@
         <v>1</v>
       </c>
       <c r="AE14" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF14" s="3">
         <v>201408</v>
@@ -12269,7 +12321,7 @@
         <v>1.2</v>
       </c>
       <c r="O15" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Q15" s="3">
         <v>201702</v>
@@ -12289,7 +12341,7 @@
         <v>1</v>
       </c>
       <c r="W15" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y15" s="3">
         <v>201803</v>
@@ -12363,7 +12415,7 @@
         <v>1</v>
       </c>
       <c r="O16" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Q16" s="3">
         <v>201702</v>
@@ -12383,7 +12435,7 @@
         <v>1.5</v>
       </c>
       <c r="W16" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y16" s="3">
         <v>201803</v>
@@ -12483,7 +12535,7 @@
         <v>2</v>
       </c>
       <c r="W17" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y17" s="3">
         <v>201803</v>
@@ -12503,7 +12555,7 @@
         <v>3</v>
       </c>
       <c r="AE17" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF17" s="3">
         <v>201411</v>
@@ -12577,7 +12629,7 @@
         <v>6</v>
       </c>
       <c r="W18" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y18" s="3">
         <v>201803</v>
@@ -12597,7 +12649,7 @@
         <v>1</v>
       </c>
       <c r="AE18" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF18" s="3">
         <v>201412</v>
@@ -12671,7 +12723,7 @@
         <v>0.2</v>
       </c>
       <c r="W19" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y19" s="3">
         <v>201803</v>
@@ -12748,7 +12800,7 @@
         <v>3.5</v>
       </c>
       <c r="O20" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Q20" s="3">
         <v>201703</v>
@@ -12768,7 +12820,7 @@
         <v>0.3</v>
       </c>
       <c r="W20" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y20" s="3">
         <v>201803</v>
@@ -12788,7 +12840,7 @@
         <v>0.2</v>
       </c>
       <c r="AE20" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF20" s="3">
         <v>201414</v>
@@ -12846,7 +12898,7 @@
         <v>4</v>
       </c>
       <c r="W21" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y21" s="3">
         <v>201803</v>
@@ -12866,7 +12918,7 @@
         <v>0.5</v>
       </c>
       <c r="AE21" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF21" s="3">
         <v>201415</v>
@@ -12921,7 +12973,7 @@
         <v>1.5</v>
       </c>
       <c r="W22" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y22" s="3">
         <v>201804</v>
@@ -12996,7 +13048,7 @@
         <v>2</v>
       </c>
       <c r="W23" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y23" s="3">
         <v>201804</v>
@@ -13071,7 +13123,7 @@
         <v>2</v>
       </c>
       <c r="W24" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y24" s="3">
         <v>201804</v>
@@ -13091,7 +13143,7 @@
         <v>3</v>
       </c>
       <c r="AE24" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF24" s="3">
         <v>201418</v>
@@ -13146,7 +13198,7 @@
         <v>1</v>
       </c>
       <c r="W25" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y25" s="3">
         <v>201804</v>
@@ -13166,7 +13218,7 @@
         <v>1</v>
       </c>
       <c r="AE25" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF25" s="3">
         <v>201419</v>
@@ -13221,7 +13273,7 @@
         <v>2</v>
       </c>
       <c r="W26" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y26" s="3">
         <v>201804</v>
@@ -13264,7 +13316,7 @@
         <v>2</v>
       </c>
       <c r="W27" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y27" s="3">
         <v>201804</v>
@@ -13284,7 +13336,7 @@
         <v>0.2</v>
       </c>
       <c r="AE27" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="28" spans="9:42">
@@ -13307,7 +13359,7 @@
         <v>50</v>
       </c>
       <c r="W28" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y28" s="3">
         <v>201804</v>
@@ -13327,7 +13379,7 @@
         <v>0.5</v>
       </c>
       <c r="AE28" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="29" spans="9:42">
@@ -13370,7 +13422,7 @@
         <v>2</v>
       </c>
       <c r="AE29" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="30" spans="9:42">
@@ -13393,7 +13445,7 @@
         <v>4</v>
       </c>
       <c r="W30" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y30" s="3">
         <v>201804</v>
@@ -13413,7 +13465,7 @@
         <v>30</v>
       </c>
       <c r="AE30" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="31" spans="9:42">
@@ -13436,7 +13488,7 @@
         <v>0.2</v>
       </c>
       <c r="W31" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y31" s="3">
         <v>201805</v>
@@ -13456,7 +13508,7 @@
         <v>2</v>
       </c>
       <c r="AE31" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="32" spans="9:42">
@@ -13479,7 +13531,7 @@
         <v>0.3</v>
       </c>
       <c r="W32" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y32" s="3">
         <v>201805</v>
@@ -13499,7 +13551,7 @@
         <v>0.4</v>
       </c>
       <c r="AE32" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="33" spans="10:35">
@@ -13522,7 +13574,7 @@
         <v>1</v>
       </c>
       <c r="W33" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y33" s="3">
         <v>201805</v>
@@ -13542,10 +13594,10 @@
         <v>0.2</v>
       </c>
       <c r="AE33" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF33" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="34" spans="10:35">
@@ -13568,7 +13620,7 @@
         <v>1.5</v>
       </c>
       <c r="W34" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y34" s="3">
         <v>201806</v>
@@ -13611,7 +13663,7 @@
         <v>2</v>
       </c>
       <c r="W35" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y35" s="3">
         <v>201806</v>
@@ -13653,7 +13705,7 @@
         <v>2</v>
       </c>
       <c r="W36" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y36" s="3">
         <v>201806</v>
@@ -13673,7 +13725,7 @@
         <v>6</v>
       </c>
       <c r="AE36" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="37" spans="10:35">
@@ -13718,7 +13770,7 @@
         <v>3</v>
       </c>
       <c r="AE37" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF37" s="29" t="s">
         <v>311</v>
@@ -13772,7 +13824,7 @@
         <v>7</v>
       </c>
       <c r="AE38" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF38" s="3" cm="1">
         <f t="array" ref="AF38:AF54">VALUE(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.TEXTJOIN(",",1,_xlfn.ANCHORARRAY(AI7)),",")))</f>
@@ -13809,7 +13861,7 @@
         <v>1</v>
       </c>
       <c r="W39" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y39" s="3">
         <v>201806</v>
@@ -13832,7 +13884,7 @@
         <v>3</v>
       </c>
       <c r="AE39" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF39" s="3">
         <v>201402</v>
@@ -13868,7 +13920,7 @@
         <v>1</v>
       </c>
       <c r="W40" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y40" s="3">
         <v>201806</v>
@@ -13888,7 +13940,7 @@
         <v>2</v>
       </c>
       <c r="AE40" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF40" s="3">
         <v>201402</v>
@@ -14036,7 +14088,7 @@
         <v>1</v>
       </c>
       <c r="W43" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y43" s="3">
         <v>201807</v>
@@ -14056,7 +14108,7 @@
         <v>6</v>
       </c>
       <c r="AE43" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF43" s="3">
         <v>201404</v>
@@ -14092,7 +14144,7 @@
         <v>1</v>
       </c>
       <c r="W44" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y44" s="3">
         <v>201807</v>
@@ -14112,7 +14164,7 @@
         <v>3</v>
       </c>
       <c r="AE44" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF44" s="3">
         <v>201404</v>
@@ -14148,7 +14200,7 @@
         <v>0.2</v>
       </c>
       <c r="W45" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y45" s="3">
         <v>201807</v>
@@ -14168,7 +14220,7 @@
         <v>4</v>
       </c>
       <c r="AE45" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF45" s="3">
         <v>201404</v>
@@ -14204,7 +14256,7 @@
         <v>0.3</v>
       </c>
       <c r="W46" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y46" s="3">
         <v>201807</v>
@@ -14224,7 +14276,7 @@
         <v>16</v>
       </c>
       <c r="AE46" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF46" s="3">
         <v>201404</v>
@@ -14260,7 +14312,7 @@
         <v>1</v>
       </c>
       <c r="W47" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y47" s="3">
         <v>201809</v>
@@ -14316,7 +14368,7 @@
         <v>1.5</v>
       </c>
       <c r="W48" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y48" s="3">
         <v>201809</v>
@@ -14375,7 +14427,7 @@
         <v>8</v>
       </c>
       <c r="W49" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y49" s="3">
         <v>201809</v>
@@ -14395,7 +14447,7 @@
         <v>1</v>
       </c>
       <c r="AE49" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF49" s="3">
         <v>201405</v>
@@ -14454,7 +14506,7 @@
         <v>11</v>
       </c>
       <c r="AE50" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF50" s="3">
         <v>201405</v>
@@ -14513,7 +14565,7 @@
         <v>2.8</v>
       </c>
       <c r="AE51" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF51" s="3">
         <v>201406</v>
@@ -14549,7 +14601,7 @@
         <v>1</v>
       </c>
       <c r="W52" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y52" s="3">
         <v>201809</v>
@@ -14569,7 +14621,7 @@
         <v>0.6</v>
       </c>
       <c r="AE52" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF52" s="3">
         <v>201407</v>
@@ -14605,7 +14657,7 @@
         <v>1</v>
       </c>
       <c r="W53" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y53" s="3">
         <v>201810</v>
@@ -14625,7 +14677,7 @@
         <v>2</v>
       </c>
       <c r="AE53" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF53" s="3">
         <v>201407</v>
@@ -14684,7 +14736,7 @@
         <v>4</v>
       </c>
       <c r="AE54" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF54" s="3">
         <v>201407</v>
@@ -14773,7 +14825,7 @@
         <v>1</v>
       </c>
       <c r="W56" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y56" s="3">
         <v>201810</v>
@@ -14793,7 +14845,7 @@
         <v>4</v>
       </c>
       <c r="AE56" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG56" s="3" t="e" cm="1">
         <f t="array" ref="AG56">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF56,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF56,$AF56))</f>
@@ -14823,7 +14875,7 @@
         <v>1</v>
       </c>
       <c r="W57" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y57" s="3">
         <v>201810</v>
@@ -14843,7 +14895,7 @@
         <v>0.1</v>
       </c>
       <c r="AE57" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG57" s="3" t="e" cm="1">
         <f t="array" ref="AG57">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF57,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF57,$AF57))</f>
@@ -14873,7 +14925,7 @@
         <v>0.2</v>
       </c>
       <c r="W58" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y58" s="3">
         <v>201810</v>
@@ -14893,7 +14945,7 @@
         <v>0.5</v>
       </c>
       <c r="AE58" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG58" s="3" t="e" cm="1">
         <f t="array" ref="AG58">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF58,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF58,$AF58))</f>
@@ -14923,7 +14975,7 @@
         <v>0.3</v>
       </c>
       <c r="W59" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y59" s="3">
         <v>201811</v>
@@ -14943,7 +14995,7 @@
         <v>0.2</v>
       </c>
       <c r="AE59" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG59" s="3" t="e" cm="1">
         <f t="array" ref="AG59">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF59,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF59,$AF59))</f>
@@ -14973,7 +15025,7 @@
         <v>1</v>
       </c>
       <c r="W60" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y60" s="3">
         <v>201811</v>
@@ -14993,7 +15045,7 @@
         <v>0.5</v>
       </c>
       <c r="AE60" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG60" s="3" t="e" cm="1">
         <f t="array" ref="AG60">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF60,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF60,$AF60))</f>
@@ -15023,7 +15075,7 @@
         <v>1.5</v>
       </c>
       <c r="W61" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y61" s="3">
         <v>201811</v>
@@ -15043,7 +15095,7 @@
         <v>6</v>
       </c>
       <c r="AE61" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG61" s="3" t="e" cm="1">
         <f t="array" ref="AG61">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF61,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF61,$AF61))</f>
@@ -15076,7 +15128,7 @@
         <v>5</v>
       </c>
       <c r="W62" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y62" s="3">
         <v>201811</v>
@@ -15096,7 +15148,7 @@
         <v>8</v>
       </c>
       <c r="AE62" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG62" s="3" t="e" cm="1">
         <f t="array" ref="AG62">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF62,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF62,$AF62))</f>
@@ -15146,7 +15198,7 @@
         <v>0.2</v>
       </c>
       <c r="AE63" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG63" s="3" t="e" cm="1">
         <f t="array" ref="AG63">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF63,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF63,$AF63))</f>
@@ -15196,7 +15248,7 @@
         <v>3</v>
       </c>
       <c r="AE64" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG64" s="3" t="e" cm="1">
         <f t="array" ref="AG64">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF64,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF64,$AF64))</f>
@@ -15226,7 +15278,7 @@
         <v>1</v>
       </c>
       <c r="W65" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y65" s="3">
         <v>201811</v>
@@ -15276,7 +15328,7 @@
         <v>1</v>
       </c>
       <c r="W66" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y66" s="3">
         <v>201811</v>
@@ -15296,7 +15348,7 @@
         <v>0.5</v>
       </c>
       <c r="AE66" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG66" s="3" t="e" cm="1">
         <f t="array" ref="AG66">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF66,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF66,$AF66))</f>
@@ -15346,7 +15398,7 @@
         <v>0.5</v>
       </c>
       <c r="AE67" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG67" s="3" t="e" cm="1">
         <f t="array" ref="AG67">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF67,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF67,$AF67))</f>
@@ -15429,7 +15481,7 @@
         <v>1</v>
       </c>
       <c r="W69" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y69" s="3">
         <v>201812</v>
@@ -15452,7 +15504,7 @@
         <v>22</v>
       </c>
       <c r="AE69" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG69" s="3" t="e" cm="1">
         <f t="array" ref="AG69">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF69,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF69,$AF69))</f>
@@ -15482,7 +15534,7 @@
         <v>1</v>
       </c>
       <c r="W70" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y70" s="3">
         <v>201812</v>
@@ -15532,7 +15584,7 @@
         <v>0.2</v>
       </c>
       <c r="W71" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y71" s="3">
         <v>201813</v>
@@ -15552,7 +15604,7 @@
         <v>3.4</v>
       </c>
       <c r="AE71" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG71" s="3" t="e" cm="1">
         <f t="array" ref="AG71">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF71,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF71,$AF71))</f>
@@ -15582,7 +15634,7 @@
         <v>0.3</v>
       </c>
       <c r="W72" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y72" s="3">
         <v>201813</v>
@@ -15602,7 +15654,7 @@
         <v>8</v>
       </c>
       <c r="AE72" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG72" s="3" t="e" cm="1">
         <f t="array" ref="AG72">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF72,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF72,$AF72))</f>
@@ -15632,7 +15684,7 @@
         <v>1</v>
       </c>
       <c r="W73" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y73" s="3">
         <v>201813</v>
@@ -15682,7 +15734,7 @@
         <v>1.5</v>
       </c>
       <c r="W74" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y74" s="3">
         <v>201813</v>
@@ -15702,7 +15754,7 @@
         <v>1</v>
       </c>
       <c r="AE74" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG74" s="3" t="e" cm="1">
         <f t="array" ref="AG74">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF74,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF74,$AF74))</f>
@@ -15735,7 +15787,7 @@
         <v>2</v>
       </c>
       <c r="W75" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y75" s="3">
         <v>201813</v>
@@ -15755,7 +15807,7 @@
         <v>0.1</v>
       </c>
       <c r="AE75" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG75" s="3" t="e" cm="1">
         <f t="array" ref="AG75">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF75,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF75,$AF75))</f>
@@ -15785,7 +15837,7 @@
         <v>0.2</v>
       </c>
       <c r="W76" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y76" s="3">
         <v>201813</v>
@@ -15805,7 +15857,7 @@
         <v>0.5</v>
       </c>
       <c r="AE76" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG76" s="3" t="e" cm="1">
         <f t="array" ref="AG76">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF76,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF76,$AF76))</f>
@@ -15835,7 +15887,7 @@
         <v>0.3</v>
       </c>
       <c r="W77" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y77" s="3">
         <v>201814</v>
@@ -15855,7 +15907,7 @@
         <v>2.9</v>
       </c>
       <c r="AE77" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG77" s="3" t="e" cm="1">
         <f t="array" ref="AG77">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF77,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF77,$AF77))</f>
@@ -15888,7 +15940,7 @@
         <v>0.1</v>
       </c>
       <c r="W78" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y78" s="3">
         <v>201814</v>
@@ -15908,7 +15960,7 @@
         <v>0.3</v>
       </c>
       <c r="AE78" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG78" s="3" t="e" cm="1">
         <f t="array" ref="AG78">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF78,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF78,$AF78))</f>
@@ -15941,7 +15993,7 @@
         <v>11</v>
       </c>
       <c r="W79" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y79" s="3">
         <v>201814</v>
@@ -15961,7 +16013,7 @@
         <v>0.27</v>
       </c>
       <c r="AE79" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG79" s="3" t="e" cm="1">
         <f t="array" ref="AG79">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF79,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF79,$AF79))</f>
@@ -15991,7 +16043,7 @@
         <v>0.2</v>
       </c>
       <c r="W80" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y80" s="3">
         <v>201814</v>
@@ -16011,7 +16063,7 @@
         <v>0.31</v>
       </c>
       <c r="AE80" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG80" s="3" t="e" cm="1">
         <f t="array" ref="AG80">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF80,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF80,$AF80))</f>
@@ -16041,7 +16093,7 @@
         <v>0.3</v>
       </c>
       <c r="W81" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y81" s="3">
         <v>201815</v>
@@ -16061,7 +16113,7 @@
         <v>4</v>
       </c>
       <c r="AE81" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG81" s="3" t="e" cm="1">
         <f t="array" ref="AG81">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF81,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF81,$AF81))</f>
@@ -16094,7 +16146,7 @@
         <v>2.5</v>
       </c>
       <c r="W82" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y82" s="3">
         <v>201815</v>
@@ -16114,7 +16166,7 @@
         <v>0.5</v>
       </c>
       <c r="AE82" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG82" s="3" t="e" cm="1">
         <f t="array" ref="AG82">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF82,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF82,$AF82))</f>
@@ -16147,7 +16199,7 @@
         <v>6</v>
       </c>
       <c r="W83" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y83" s="3">
         <v>201815</v>
@@ -16167,7 +16219,7 @@
         <v>0.27</v>
       </c>
       <c r="AE83" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG83" s="3" t="e" cm="1">
         <f t="array" ref="AG83">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF83,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF83,$AF83))</f>
@@ -16197,7 +16249,7 @@
         <v>0.1</v>
       </c>
       <c r="W84" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y84" s="3">
         <v>201815</v>
@@ -16217,7 +16269,7 @@
         <v>0.31</v>
       </c>
       <c r="AE84" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG84" s="3" t="e" cm="1">
         <f t="array" ref="AG84">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF84,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF84,$AF84))</f>
@@ -16367,7 +16419,7 @@
         <v>1</v>
       </c>
       <c r="AE87" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG87" s="3" t="e" cm="1">
         <f t="array" ref="AG87">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF87,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF87,$AF87))</f>
@@ -16397,7 +16449,7 @@
         <v>50</v>
       </c>
       <c r="W88" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y88" s="3">
         <v>201850</v>
@@ -16417,7 +16469,7 @@
         <v>1</v>
       </c>
       <c r="AE88" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG88" s="3" t="e" cm="1">
         <f t="array" ref="AG88">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF88,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF88,$AF88))</f>
@@ -16447,7 +16499,7 @@
         <v>0.1</v>
       </c>
       <c r="W89" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y89" s="3">
         <v>201850</v>
@@ -16467,7 +16519,7 @@
         <v>5</v>
       </c>
       <c r="AE89" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG89" s="3" t="e" cm="1">
         <f t="array" ref="AG89">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF89,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF89,$AF89))</f>
@@ -16517,7 +16569,7 @@
         <v>3</v>
       </c>
       <c r="AE90" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG90" s="3" t="e" cm="1">
         <f t="array" ref="AG90">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF90,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF90,$AF90))</f>
@@ -16567,7 +16619,7 @@
         <v>10</v>
       </c>
       <c r="AE91" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG91" s="3" t="e" cm="1">
         <f t="array" ref="AG91">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF91,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF91,$AF91))</f>
@@ -16617,7 +16669,7 @@
         <v>0.15</v>
       </c>
       <c r="AE92" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG92" s="3" t="e" cm="1">
         <f t="array" ref="AG92">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF92,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF92,$AF92))</f>
@@ -16647,7 +16699,7 @@
         <v>50</v>
       </c>
       <c r="W93" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y93" s="3">
         <v>201860</v>
@@ -16727,7 +16779,7 @@
         <v>2</v>
       </c>
       <c r="AE95" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG95" s="3" t="e" cm="1">
         <f t="array" ref="AG95">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF95,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF95,$AF95))</f>
@@ -16757,7 +16809,7 @@
         <v>1</v>
       </c>
       <c r="AE96" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG96" s="3" t="e" cm="1">
         <f t="array" ref="AG96">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF96,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF96,$AF96))</f>
@@ -16787,7 +16839,7 @@
         <v>3</v>
       </c>
       <c r="AE97" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG97" s="3" t="e" cm="1">
         <f t="array" ref="AG97">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF97,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF97,$AF97))</f>
@@ -16817,7 +16869,7 @@
         <v>4</v>
       </c>
       <c r="AE98" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG98" s="3" t="e" cm="1">
         <f t="array" ref="AG98">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF98,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF98,$AF98))</f>
@@ -16847,7 +16899,7 @@
         <v>8</v>
       </c>
       <c r="AE99" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG99" s="3" t="e" cm="1">
         <f t="array" ref="AG99">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF99,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF99,$AF99))</f>
@@ -16877,7 +16929,7 @@
         <v>16</v>
       </c>
       <c r="AE100" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG100" s="3" t="e" cm="1">
         <f t="array" ref="AG100">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF100,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF100,$AF100))</f>
@@ -16907,7 +16959,7 @@
         <v>3</v>
       </c>
       <c r="AE101" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG101" s="3" t="e" cm="1">
         <f t="array" ref="AG101">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF101,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF101,$AF101))</f>
@@ -16997,7 +17049,7 @@
         <v>1</v>
       </c>
       <c r="AE104" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG104" s="3" t="e" cm="1">
         <f t="array" ref="AG104">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF104,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF104,$AF104))</f>
@@ -17027,7 +17079,7 @@
         <v>1</v>
       </c>
       <c r="AE105" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG105" s="3" t="e" cm="1">
         <f t="array" ref="AG105">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF105,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF105,$AF105))</f>
@@ -17057,7 +17109,7 @@
         <v>2</v>
       </c>
       <c r="AE106" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG106" s="3" t="e" cm="1">
         <f t="array" ref="AG106">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF106,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF106,$AF106))</f>
@@ -17087,7 +17139,7 @@
         <v>0.6</v>
       </c>
       <c r="AE107" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG107" s="3" t="e" cm="1">
         <f t="array" ref="AG107">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF107,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF107,$AF107))</f>
@@ -17117,7 +17169,7 @@
         <v>0.4</v>
       </c>
       <c r="AE108" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG108" s="3" t="e" cm="1">
         <f t="array" ref="AG108">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF108,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF108,$AF108))</f>
@@ -17147,7 +17199,7 @@
         <v>3</v>
       </c>
       <c r="AE109" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG109" s="3" t="e" cm="1">
         <f t="array" ref="AG109">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF109,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF109,$AF109))</f>
@@ -17177,7 +17229,7 @@
         <v>3</v>
       </c>
       <c r="AE110" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG110" s="3" t="e" cm="1">
         <f t="array" ref="AG110">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF110,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF110,$AF110))</f>
@@ -17207,7 +17259,7 @@
         <v>0.58</v>
       </c>
       <c r="AE111" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG111" s="3" t="e" cm="1">
         <f t="array" ref="AG111">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF111,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF111,$AF111))</f>
@@ -17273,7 +17325,7 @@
         <v>10</v>
       </c>
       <c r="AE113" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG113" s="3" t="e" cm="1">
         <f t="array" ref="AG113">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF113,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF113,$AF113))</f>
@@ -17333,7 +17385,7 @@
         <v>0.31</v>
       </c>
       <c r="AE115" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG115" s="3" t="e" cm="1">
         <f t="array" ref="AG115">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF115,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF115,$AF115))</f>
@@ -17399,7 +17451,7 @@
         <v>22</v>
       </c>
       <c r="AE117" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG117" s="3" t="e" cm="1">
         <f t="array" ref="AG117">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF117,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF117,$AF117))</f>
@@ -17519,7 +17571,7 @@
         <v>1</v>
       </c>
       <c r="AE121" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG121" s="3" t="e" cm="1">
         <f t="array" ref="AG121">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF121,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF121,$AF121))</f>
@@ -17549,7 +17601,7 @@
         <v>11</v>
       </c>
       <c r="AE122" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG122" s="3" t="e" cm="1">
         <f t="array" ref="AG122">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF122,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF122,$AF122))</f>
@@ -17579,7 +17631,7 @@
         <v>2.8</v>
       </c>
       <c r="AE123" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG123" s="3" t="e" cm="1">
         <f t="array" ref="AG123">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF123,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF123,$AF123))</f>
@@ -17609,7 +17661,7 @@
         <v>0.6</v>
       </c>
       <c r="AE124" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG124" s="3" t="e" cm="1">
         <f t="array" ref="AG124">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF124,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF124,$AF124))</f>
@@ -17639,7 +17691,7 @@
         <v>0.58</v>
       </c>
       <c r="AE125" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG125" s="3" t="e" cm="1">
         <f t="array" ref="AG125">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF125,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF125,$AF125))</f>
@@ -17705,7 +17757,7 @@
         <v>10</v>
       </c>
       <c r="AE127" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AG127" s="3" t="e" cm="1">
         <f t="array" ref="AG127">INDEX(TRANSPOSE(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(AF127,$AF$7:$AF$18,$AG$7:$AG$18),";")),COUNTIF($AF$38:$AF127,$AF127))</f>
@@ -17804,7 +17856,7 @@
         <v>3</v>
       </c>
       <c r="AE131" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="132" spans="25:31">
@@ -17826,7 +17878,7 @@
         <v>1</v>
       </c>
       <c r="AE132" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="133" spans="25:31">
@@ -17873,7 +17925,7 @@
         <v>0.2</v>
       </c>
       <c r="AE134" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="135" spans="25:31">
@@ -17895,7 +17947,7 @@
         <v>0.5</v>
       </c>
       <c r="AE135" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -20875,7 +20927,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{a53faaef-6bee-441c-a0d3-4a3c263dbab7}</x14:id>
+          <x14:id>{f5b456f4-8295-4178-b25e-fd0bdce02cc2}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -20888,7 +20940,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{a53faaef-6bee-441c-a0d3-4a3c263dbab7}">
+          <x14:cfRule type="dataBar" id="{f5b456f4-8295-4178-b25e-fd0bdce02cc2}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>-10</xm:f>

</xml_diff>

<commit_message>
--Add 1815 1. 跳跃射击。
</commit_message>
<xml_diff>
--- a/Assets/Tables/table_enemy.xlsx
+++ b/Assets/Tables/table_enemy.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1391" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="465">
   <si>
     <t>id</t>
   </si>
@@ -1076,6 +1076,18 @@
   </si>
   <si>
     <t>JUMP_CD=0.58;ATK_AREA=1,2;JUMP_VELOCITY_X_MAX=20;JUMP_HEIGHT_AREA=1,2</t>
+  </si>
+  <si>
+    <t>跳跃远程</t>
+  </si>
+  <si>
+    <t>monster_201810_Lake_Swamp</t>
+  </si>
+  <si>
+    <t>BT_Common_JumpShoot</t>
+  </si>
+  <si>
+    <t>JUMP_CD=0.58;ATTACK_DIS=5;JUMP_VELOCITY_X_MAX=20;JUMP_HEIGHT_AREA=1,2;BEFORE_ATTACK_SEC=0.6;AFTER_ATTACK_SEC=0.4;RUNNING_FIRE_COUNT=3</t>
   </si>
   <si>
     <t>parm_key</t>
@@ -3491,7 +3503,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AT85" sqref="AT85"/>
+      <selection pane="bottomRight" activeCell="AT86" sqref="AT86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
@@ -10810,7 +10822,6 @@
       <c r="A82" s="24">
         <v>209100</v>
       </c>
-      <c r="B82" s="24"/>
       <c r="D82" s="25" t="s">
         <v>235</v>
       </c>
@@ -10851,7 +10862,6 @@
       <c r="AA82" s="69" t="s">
         <v>237</v>
       </c>
-      <c r="AB82" s="50"/>
       <c r="AC82" s="69" t="s">
         <v>238</v>
       </c>
@@ -10878,9 +10888,6 @@
       </c>
       <c r="AK82" s="51" t="s">
         <v>82</v>
-      </c>
-      <c r="AM82" s="51" t="s">
-        <v>183</v>
       </c>
       <c r="AN82" s="68">
         <v>0</v>
@@ -10988,7 +10995,6 @@
       <c r="A84" s="24">
         <v>209102</v>
       </c>
-      <c r="B84" s="24"/>
       <c r="D84" s="25" t="s">
         <v>244</v>
       </c>
@@ -11022,7 +11028,6 @@
       <c r="AA84" s="69" t="s">
         <v>237</v>
       </c>
-      <c r="AB84" s="50"/>
       <c r="AC84" s="69" t="s">
         <v>246</v>
       </c>
@@ -11058,8 +11063,6 @@
       <c r="A85" s="24">
         <v>209103</v>
       </c>
-      <c r="B85" s="24"/>
-      <c r="C85" s="25"/>
       <c r="D85" s="25" t="s">
         <v>248</v>
       </c>
@@ -11075,7 +11078,6 @@
       <c r="J85" s="24">
         <v>7.12</v>
       </c>
-      <c r="K85" s="24"/>
       <c r="M85" s="24" t="s">
         <v>245</v>
       </c>
@@ -11085,14 +11087,12 @@
       <c r="AA85" s="69" t="s">
         <v>237</v>
       </c>
-      <c r="AB85" s="50"/>
       <c r="AC85" s="69" t="s">
         <v>249</v>
       </c>
       <c r="AE85" s="24">
         <v>0.05</v>
       </c>
-      <c r="AF85" s="24"/>
       <c r="AG85" t="s">
         <v>228</v>
       </c>
@@ -11108,9 +11108,6 @@
       <c r="AK85" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="AM85" s="51" t="s">
-        <v>183</v>
-      </c>
       <c r="AN85" s="24">
         <v>0</v>
       </c>
@@ -11122,7 +11119,66 @@
       </c>
     </row>
     <row r="86" spans="1:46">
-      <c r="H86" s="67"/>
+      <c r="A86" s="24">
+        <v>209104</v>
+      </c>
+      <c r="D86" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="G86" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H86" s="67">
+        <v>3000</v>
+      </c>
+      <c r="I86" s="24">
+        <v>0</v>
+      </c>
+      <c r="J86" s="24">
+        <v>7.12</v>
+      </c>
+      <c r="M86" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="N86" s="47">
+        <v>3</v>
+      </c>
+      <c r="AA86" s="69" t="s">
+        <v>252</v>
+      </c>
+      <c r="AC86" s="69" t="s">
+        <v>253</v>
+      </c>
+      <c r="AD86" s="67">
+        <v>201810</v>
+      </c>
+      <c r="AE86" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="AG86" t="s">
+        <v>228</v>
+      </c>
+      <c r="AH86" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI86" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ86" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK86" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN86" s="24">
+        <v>0</v>
+      </c>
+      <c r="AO86" s="24" t="s">
+        <v>236</v>
+      </c>
+      <c r="AT86" t="s">
+        <v>254</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -11185,19 +11241,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>0</v>
@@ -11206,19 +11262,19 @@
         <v>1</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="Q3" s="5" t="s">
         <v>0</v>
@@ -11227,19 +11283,19 @@
         <v>1</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="Y3" s="5" t="s">
         <v>0</v>
@@ -11248,19 +11304,19 @@
         <v>1</v>
       </c>
       <c r="AA3" s="5" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="AB3" s="5" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="AC3" s="5" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="AD3" s="5" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="AE3" s="5" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:42">
@@ -11279,10 +11335,10 @@
         <v>毒刺果实丛</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="M4" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11302,7 +11358,7 @@
         <v>涂涂鸟</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="U4" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11322,7 +11378,7 @@
         <v>金鱼</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="AC4" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11351,7 +11407,7 @@
         <v>毒刺果实丛</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="M5" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11371,7 +11427,7 @@
         <v>涂涂鸟</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="U5" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11391,10 +11447,10 @@
         <v>金鱼</v>
       </c>
       <c r="AA5" s="3" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="AB5" s="5" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="AC5" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11423,7 +11479,7 @@
         <v>毒刺果实丛</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="M6" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11443,7 +11499,7 @@
         <v>涂涂鸟</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="U6" s="92" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11463,7 +11519,7 @@
         <v>金鱼</v>
       </c>
       <c r="AA6" s="3" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="AC6" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11476,16 +11532,16 @@
         <v>236</v>
       </c>
       <c r="AF6" s="29" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="AG6" s="29" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="AH6" s="29" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="AI6" s="29" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="7" spans="1:42">
@@ -11504,7 +11560,7 @@
         <v>画中仙</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="M7" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11524,7 +11580,7 @@
         <v>涂涂鸟</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="U7" s="5" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11544,7 +11600,7 @@
         <v>金鱼</v>
       </c>
       <c r="AA7" s="3" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="AC7" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11606,7 +11662,7 @@
         <v>画中仙</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="M8" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11626,7 +11682,7 @@
         <v>涂涂鸟</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="U8" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11646,10 +11702,10 @@
         <v>金鱼</v>
       </c>
       <c r="AA8" s="3" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="AB8" s="5" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="AC8" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11665,7 +11721,7 @@
         <v>201402</v>
       </c>
       <c r="AG8" s="40" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="AH8" s="3">
         <f t="shared" ref="AH8:AH25" si="0">IFERROR(COLUMNS(_xlfn.TEXTSPLIT(AG8,";")),0)</f>
@@ -11712,7 +11768,7 @@
         <v>画中仙</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="M9" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11732,7 +11788,7 @@
         <v>涂涂鸟</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="U9" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11752,7 +11808,7 @@
         <v>金鱼</v>
       </c>
       <c r="AA9" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AC9" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11813,7 +11869,7 @@
         <v>画中仙</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="M10" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11833,7 +11889,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="U10" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11853,7 +11909,7 @@
         <v>金鱼</v>
       </c>
       <c r="AA10" s="3" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="AC10" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11869,7 +11925,7 @@
         <v>201404</v>
       </c>
       <c r="AG10" s="40" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AH10" s="3">
         <f t="shared" si="0"/>
@@ -11916,7 +11972,7 @@
         <v>画中仙</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="M11" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11936,7 +11992,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="U11" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11956,10 +12012,10 @@
         <v>金鱼</v>
       </c>
       <c r="AA11" s="3" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AB11" s="5" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="AC11" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11975,7 +12031,7 @@
         <v>201405</v>
       </c>
       <c r="AG11" s="40" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="AH11" s="3">
         <f t="shared" si="0"/>
@@ -12022,7 +12078,7 @@
         <v>画中仙</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="M12" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12042,7 +12098,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S12" s="3" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="U12" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12062,10 +12118,10 @@
         <v>金鱼</v>
       </c>
       <c r="AA12" s="3" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="AB12" s="5" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="AC12" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12081,7 +12137,7 @@
         <v>201406</v>
       </c>
       <c r="AG12" s="40" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="AH12" s="3">
         <f t="shared" si="0"/>
@@ -12121,7 +12177,7 @@
         <v>画中仙</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="M13" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12141,7 +12197,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S13" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="U13" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12161,7 +12217,7 @@
         <v>金鱼泡泡</v>
       </c>
       <c r="AA13" s="3" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="AC13" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12177,7 +12233,7 @@
         <v>201407</v>
       </c>
       <c r="AG13" s="40" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="AH13" s="3">
         <f t="shared" si="0"/>
@@ -12217,7 +12273,7 @@
         <v>画中仙</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="M14" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12237,7 +12293,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S14" s="3" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="U14" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12257,7 +12313,7 @@
         <v>金鱼泡泡</v>
       </c>
       <c r="AA14" s="3" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="AC14" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12311,7 +12367,7 @@
         <v>鱼妖</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="M15" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12331,7 +12387,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="U15" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12351,7 +12407,7 @@
         <v>海藻小妖</v>
       </c>
       <c r="AA15" s="3" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="AC15" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12405,7 +12461,7 @@
         <v>鱼妖</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="M16" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12425,7 +12481,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="U16" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12445,10 +12501,10 @@
         <v>海藻小妖</v>
       </c>
       <c r="AA16" s="3" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="AB16" s="5" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="AC16" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12502,10 +12558,10 @@
         <v>鬼瓮</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="M17" s="5" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12525,7 +12581,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="U17" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12545,7 +12601,7 @@
         <v>海藻小妖</v>
       </c>
       <c r="AA17" s="3" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="AC17" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12599,7 +12655,7 @@
         <v>鬼狰</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="M18" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12619,7 +12675,7 @@
         <v>巨牙蝎</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="U18" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12639,7 +12695,7 @@
         <v>海藻小妖</v>
       </c>
       <c r="AA18" s="3" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="AC18" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12693,7 +12749,7 @@
         <v>鬼狰</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="M19" s="5" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12713,7 +12769,7 @@
         <v>巨牙蝎</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="U19" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12733,10 +12789,10 @@
         <v>海藻小妖</v>
       </c>
       <c r="AA19" s="3" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="AB19" s="5" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="AC19" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12790,7 +12846,7 @@
         <v>鬼狰</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="M20" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12810,7 +12866,7 @@
         <v>巨牙蝎</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="U20" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12830,7 +12886,7 @@
         <v>海藻小妖</v>
       </c>
       <c r="AA20" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AC20" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12885,10 +12941,10 @@
         <v>巨牙蝎</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="T21" s="5" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="U21" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12908,7 +12964,7 @@
         <v>海藻小妖</v>
       </c>
       <c r="AA21" s="3" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="AC21" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12963,7 +13019,7 @@
         <v>巨牙蝎</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="U22" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12983,7 +13039,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA22" s="3" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="AC22" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13038,7 +13094,7 @@
         <v>巨牙蝎</v>
       </c>
       <c r="S23" s="3" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="U23" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13058,7 +13114,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA23" s="3" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="AC23" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13113,7 +13169,7 @@
         <v>巨牙蝎</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="U24" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13133,7 +13189,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA24" s="3" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="AC24" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13188,7 +13244,7 @@
         <v>巨型石头人</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="U25" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13208,7 +13264,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA25" s="3" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="AC25" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13263,7 +13319,7 @@
         <v>巨型石头人</v>
       </c>
       <c r="S26" s="3" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="U26" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13283,7 +13339,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA26" s="3" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="AC26" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13306,7 +13362,7 @@
         <v>巨型石头人</v>
       </c>
       <c r="S27" s="3" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="U27" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13326,7 +13382,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA27" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AC27" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13349,7 +13405,7 @@
         <v>巨型石头人</v>
       </c>
       <c r="S28" s="3" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="U28" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13369,7 +13425,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA28" s="3" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="AC28" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13392,7 +13448,7 @@
         <v>巨型石头人</v>
       </c>
       <c r="S29" s="3" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="U29" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13412,7 +13468,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA29" s="3" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="AC29" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13435,7 +13491,7 @@
         <v>小石头人</v>
       </c>
       <c r="S30" s="3" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="U30" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13455,7 +13511,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA30" s="3" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="AC30" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13478,7 +13534,7 @@
         <v>小石头人</v>
       </c>
       <c r="S31" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="U31" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13498,7 +13554,7 @@
         <v>似目草</v>
       </c>
       <c r="AA31" s="3" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="AC31" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13521,7 +13577,7 @@
         <v>小石头人</v>
       </c>
       <c r="S32" s="3" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="U32" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13541,7 +13597,7 @@
         <v>似目草</v>
       </c>
       <c r="AA32" s="3" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="AC32" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13564,7 +13620,7 @@
         <v>小石头人</v>
       </c>
       <c r="S33" s="3" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="U33" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13584,7 +13640,7 @@
         <v>似目草</v>
       </c>
       <c r="AA33" s="5" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="AC33" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13610,7 +13666,7 @@
         <v>小石头人</v>
       </c>
       <c r="S34" s="3" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="U34" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13630,7 +13686,7 @@
         <v>脑型大水母</v>
       </c>
       <c r="AA34" s="3" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="AC34" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13652,7 +13708,7 @@
         <v>小石头人</v>
       </c>
       <c r="S35" s="3" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="T35" s="5"/>
       <c r="U35" s="3" t="str">
@@ -13673,7 +13729,7 @@
         <v>脑型大水母</v>
       </c>
       <c r="AA35" s="3" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="AC35" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13695,7 +13751,7 @@
         <v>小石头人</v>
       </c>
       <c r="S36" s="3" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="U36" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13715,7 +13771,7 @@
         <v>脑型大水母</v>
       </c>
       <c r="AA36" s="3" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="AC36" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13737,10 +13793,10 @@
         <v>大盾守卫</v>
       </c>
       <c r="S37" s="3" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="T37" s="5" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="U37" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13760,7 +13816,7 @@
         <v>脑型大水母</v>
       </c>
       <c r="AA37" s="3" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="AC37" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13773,13 +13829,13 @@
         <v>236</v>
       </c>
       <c r="AF37" s="29" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="AG37" s="29" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="AH37" s="29" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="38" spans="10:35">
@@ -13791,10 +13847,10 @@
         <v>大盾守卫</v>
       </c>
       <c r="S38" s="3" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="T38" s="5" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="U38" s="5" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13814,7 +13870,7 @@
         <v>脑型大水母</v>
       </c>
       <c r="AA38" s="3" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="AC38" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13851,7 +13907,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S39" s="3" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="U39" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13871,10 +13927,10 @@
         <v>脑型大水母</v>
       </c>
       <c r="AA39" s="3" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="AB39" s="5" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="AC39" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13910,7 +13966,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S40" s="3" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="U40" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13930,7 +13986,7 @@
         <v>脑型大水母</v>
       </c>
       <c r="AA40" s="3" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="AC40" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13966,7 +14022,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S41" s="3" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="U41" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13986,7 +14042,7 @@
         <v>针刺小水母</v>
       </c>
       <c r="AA41" s="3" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="AC41" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14022,7 +14078,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S42" s="3" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="U42" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14042,7 +14098,7 @@
         <v>针刺小水母</v>
       </c>
       <c r="AA42" s="3" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="AC42" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14078,7 +14134,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S43" s="3" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="U43" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14098,7 +14154,7 @@
         <v>针刺小水母</v>
       </c>
       <c r="AA43" s="3" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="AC43" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14134,7 +14190,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S44" s="3" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="U44" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14154,7 +14210,7 @@
         <v>针刺小水母</v>
       </c>
       <c r="AA44" s="3" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="AC44" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14190,7 +14246,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S45" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="U45" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14210,7 +14266,7 @@
         <v>针刺小水母</v>
       </c>
       <c r="AA45" s="3" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="AC45" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14246,7 +14302,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S46" s="3" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="U46" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14266,7 +14322,7 @@
         <v>针刺小水母</v>
       </c>
       <c r="AA46" s="3" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="AC46" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14302,7 +14358,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S47" s="3" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="U47" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14322,7 +14378,7 @@
         <v>印花水母</v>
       </c>
       <c r="AA47" s="3" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="AC47" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14358,7 +14414,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S48" s="3" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="U48" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14378,7 +14434,7 @@
         <v>印花水母</v>
       </c>
       <c r="AA48" s="3" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="AC48" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14414,10 +14470,10 @@
         <v>大盾守卫</v>
       </c>
       <c r="S49" s="3" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="T49" s="5" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="U49" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14437,7 +14493,7 @@
         <v>印花水母</v>
       </c>
       <c r="AA49" s="3" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="AC49" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14473,10 +14529,10 @@
         <v>基础守卫</v>
       </c>
       <c r="S50" s="3" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="T50" s="5" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="U50" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14496,7 +14552,7 @@
         <v>印花水母</v>
       </c>
       <c r="AA50" s="3" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="AC50" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14532,10 +14588,10 @@
         <v>基础守卫</v>
       </c>
       <c r="S51" s="3" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="T51" s="5" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="U51" s="5" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14555,7 +14611,7 @@
         <v>印花水母</v>
       </c>
       <c r="AA51" s="3" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="AC51" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14591,7 +14647,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S52" s="3" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="U52" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14611,7 +14667,7 @@
         <v>印花水母</v>
       </c>
       <c r="AA52" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AC52" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14647,7 +14703,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S53" s="3" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="U53" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14667,7 +14723,7 @@
         <v>混沌沼泽怪</v>
       </c>
       <c r="AA53" s="3" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="AC53" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14703,10 +14759,10 @@
         <v>基础守卫</v>
       </c>
       <c r="S54" s="3" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="T54" s="5" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="U54" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14726,7 +14782,7 @@
         <v>混沌沼泽怪</v>
       </c>
       <c r="AA54" s="3" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="AC54" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14762,10 +14818,10 @@
         <v>基础守卫</v>
       </c>
       <c r="S55" s="3" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="T55" s="5" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="U55" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14785,7 +14841,7 @@
         <v>混沌沼泽怪</v>
       </c>
       <c r="AA55" s="3" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="AC55" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14815,7 +14871,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S56" s="3" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="U56" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14835,7 +14891,7 @@
         <v>混沌沼泽怪</v>
       </c>
       <c r="AA56" s="3" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="AC56" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14865,7 +14921,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S57" s="3" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="U57" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14885,7 +14941,7 @@
         <v>混沌沼泽怪</v>
       </c>
       <c r="AA57" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AC57" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14915,7 +14971,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S58" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="U58" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14935,7 +14991,7 @@
         <v>混沌沼泽怪</v>
       </c>
       <c r="AA58" s="3" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="AC58" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14965,7 +15021,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S59" s="3" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="U59" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14985,7 +15041,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA59" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AC59" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15015,7 +15071,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S60" s="3" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="U60" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15035,7 +15091,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA60" s="3" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="AC60" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15065,7 +15121,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S61" s="3" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="U61" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15085,7 +15141,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA61" s="3" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="AC61" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15115,10 +15171,10 @@
         <v>基础守卫</v>
       </c>
       <c r="S62" s="3" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="T62" s="5" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="U62" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15138,7 +15194,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA62" s="3" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="AC62" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15168,7 +15224,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S63" s="3" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="U63" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15188,7 +15244,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA63" s="3" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="AC63" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15218,7 +15274,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S64" s="3" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="U64" s="5" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15238,7 +15294,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA64" s="3" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="AC64" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15268,7 +15324,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S65" s="3" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="U65" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15288,7 +15344,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA65" s="3" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="AC65" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15318,7 +15374,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S66" s="3" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="U66" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15338,7 +15394,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA66" s="3" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="AC66" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15368,7 +15424,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S67" s="3" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="U67" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15388,7 +15444,7 @@
         <v/>
       </c>
       <c r="AA67" s="3" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="AC67" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15418,7 +15474,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S68" s="3" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="U68" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15438,10 +15494,10 @@
         <v/>
       </c>
       <c r="AA68" s="3" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="AB68" s="5" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="AC68" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15471,7 +15527,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S69" s="3" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="U69" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15491,10 +15547,10 @@
         <v/>
       </c>
       <c r="AA69" s="3" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="AB69" s="5" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="AC69" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15524,7 +15580,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S70" s="3" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="U70" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15544,7 +15600,7 @@
         <v/>
       </c>
       <c r="AA70" s="3" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="AC70" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15574,7 +15630,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S71" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="U71" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15594,7 +15650,7 @@
         <v>贝壳乌贼</v>
       </c>
       <c r="AA71" s="3" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="AC71" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15624,7 +15680,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S72" s="3" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="U72" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15644,7 +15700,7 @@
         <v>贝壳乌贼</v>
       </c>
       <c r="AA72" s="3" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="AC72" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15674,7 +15730,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S73" s="3" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="U73" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15694,7 +15750,7 @@
         <v>贝壳乌贼</v>
       </c>
       <c r="AA73" s="3" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="AC73" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15724,7 +15780,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S74" s="3" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="U74" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15744,7 +15800,7 @@
         <v>贝壳乌贼</v>
       </c>
       <c r="AA74" s="3" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="AC74" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15774,10 +15830,10 @@
         <v>双刀守卫</v>
       </c>
       <c r="S75" s="3" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="T75" s="5" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="U75" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15797,7 +15853,7 @@
         <v>贝壳乌贼</v>
       </c>
       <c r="AA75" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AC75" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15827,7 +15883,7 @@
         <v>大仙人掌</v>
       </c>
       <c r="S76" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="U76" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15847,7 +15903,7 @@
         <v>贝壳乌贼</v>
       </c>
       <c r="AA76" s="3" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="AC76" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15877,7 +15933,7 @@
         <v>大仙人掌</v>
       </c>
       <c r="S77" s="3" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="U77" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15897,7 +15953,7 @@
         <v>弱小螃蟹</v>
       </c>
       <c r="AA77" s="3" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="AC77" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15927,10 +15983,10 @@
         <v>大仙人掌</v>
       </c>
       <c r="S78" s="3" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="T78" s="5" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="U78" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15950,7 +16006,7 @@
         <v>弱小螃蟹</v>
       </c>
       <c r="AA78" s="3" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="AC78" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15980,10 +16036,10 @@
         <v>大仙人掌</v>
       </c>
       <c r="S79" s="3" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="T79" s="5" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="U79" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16003,7 +16059,7 @@
         <v>弱小螃蟹</v>
       </c>
       <c r="AA79" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AC79" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16033,7 +16089,7 @@
         <v>小仙人掌</v>
       </c>
       <c r="S80" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="U80" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16053,7 +16109,7 @@
         <v>弱小螃蟹</v>
       </c>
       <c r="AA80" s="3" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="AC80" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16083,7 +16139,7 @@
         <v>小仙人掌</v>
       </c>
       <c r="S81" s="3" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="U81" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16103,7 +16159,7 @@
         <v>大钳螃蟹</v>
       </c>
       <c r="AA81" s="3" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="AC81" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16133,10 +16189,10 @@
         <v>小仙人掌</v>
       </c>
       <c r="S82" s="3" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="T82" s="5" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="U82" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16156,7 +16212,7 @@
         <v>大钳螃蟹</v>
       </c>
       <c r="AA82" s="3" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="AC82" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16186,10 +16242,10 @@
         <v>小仙人掌</v>
       </c>
       <c r="S83" s="3" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="T83" s="5" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="U83" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16209,7 +16265,7 @@
         <v>大钳螃蟹</v>
       </c>
       <c r="AA83" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AC83" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16239,7 +16295,7 @@
         <v>大风滚草</v>
       </c>
       <c r="S84" s="3" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="U84" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16259,7 +16315,7 @@
         <v>大钳螃蟹</v>
       </c>
       <c r="AA84" s="3" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="AC84" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16289,7 +16345,7 @@
         <v>大风滚草</v>
       </c>
       <c r="S85" s="3" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="U85" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16309,7 +16365,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA85" s="3" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="AC85" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16339,7 +16395,7 @@
         <v>大风滚草</v>
       </c>
       <c r="S86" s="3" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="U86" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16359,7 +16415,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA86" s="3" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="AC86" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16389,7 +16445,7 @@
         <v>大风滚草</v>
       </c>
       <c r="S87" s="3" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="U87" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16409,7 +16465,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA87" s="3" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="AC87" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16439,7 +16495,7 @@
         <v>大风滚草</v>
       </c>
       <c r="S88" s="3" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="U88" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16459,7 +16515,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA88" s="3" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="AC88" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16489,7 +16545,7 @@
         <v>小风滚草</v>
       </c>
       <c r="S89" s="3" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="U89" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16509,7 +16565,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA89" s="3" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="AC89" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16539,7 +16595,7 @@
         <v>小风滚草</v>
       </c>
       <c r="S90" s="3" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="U90" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16559,7 +16615,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA90" s="3" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="AC90" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16589,7 +16645,7 @@
         <v>小风滚草</v>
       </c>
       <c r="S91" s="3" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="U91" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16609,7 +16665,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA91" s="3" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AC91" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16639,7 +16695,7 @@
         <v>小风滚草</v>
       </c>
       <c r="S92" s="3" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="U92" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16659,7 +16715,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA92" s="3" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="AC92" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16689,7 +16745,7 @@
         <v>小风滚草</v>
       </c>
       <c r="S93" s="3" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="U93" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16709,7 +16765,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA93" s="3" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="AC93" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16739,7 +16795,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA94" s="3" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="AC94" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16769,7 +16825,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA95" s="3" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="AC95" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16799,7 +16855,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA96" s="3" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="AC96" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16829,7 +16885,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA97" s="3" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="AC97" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16859,7 +16915,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA98" s="3" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="AC98" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16889,7 +16945,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA99" s="3" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="AC99" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16919,7 +16975,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA100" s="3" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="AC100" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16949,7 +17005,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA101" s="3" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="AC101" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16979,7 +17035,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA102" s="3" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="AC102" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17009,7 +17065,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA103" s="3" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="AC103" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17039,7 +17095,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA104" s="3" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="AC104" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17069,7 +17125,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA105" s="3" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="AC105" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17099,7 +17155,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA106" s="3" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="AC106" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17129,7 +17185,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA107" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AC107" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17159,7 +17215,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA108" s="3" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="AC108" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17189,7 +17245,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA109" s="3" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="AC109" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17219,7 +17275,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA110" s="3" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="AC110" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17249,7 +17305,7 @@
         <v>聒噪海贝</v>
       </c>
       <c r="AA111" s="3" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="AC111" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17279,10 +17335,10 @@
         <v>聒噪海贝</v>
       </c>
       <c r="AA112" s="3" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="AB112" s="5" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="AC112" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17312,10 +17368,10 @@
         <v>聒噪海贝</v>
       </c>
       <c r="AA113" s="3" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="AB113" s="5" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="AC113" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17345,7 +17401,7 @@
         <v>聒噪海贝</v>
       </c>
       <c r="AA114" s="3" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="AC114" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17375,7 +17431,7 @@
         <v>凶猛海贝</v>
       </c>
       <c r="AA115" s="3" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="AC115" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17405,10 +17461,10 @@
         <v>凶猛海贝</v>
       </c>
       <c r="AA116" s="3" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="AB116" s="5" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="AC116" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17438,10 +17494,10 @@
         <v>凶猛海贝</v>
       </c>
       <c r="AA117" s="3" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="AB117" s="5" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="AC117" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17471,7 +17527,7 @@
         <v>凶猛海贝</v>
       </c>
       <c r="AA118" s="3" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="AC118" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17501,7 +17557,7 @@
         <v>小·印花水母</v>
       </c>
       <c r="AA119" s="41" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="AC119" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17531,7 +17587,7 @@
         <v>小·印花水母</v>
       </c>
       <c r="AA120" s="41" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="AC120" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17561,7 +17617,7 @@
         <v>小·印花水母</v>
       </c>
       <c r="AA121" s="41" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="AC121" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17591,7 +17647,7 @@
         <v>小·印花水母</v>
       </c>
       <c r="AA122" s="41" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="AC122" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17621,7 +17677,7 @@
         <v>小·印花水母</v>
       </c>
       <c r="AA123" s="41" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="AC123" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17651,7 +17707,7 @@
         <v>小·印花水母</v>
       </c>
       <c r="AA124" s="41" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AC124" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17681,7 +17737,7 @@
         <v>小·聒噪海贝</v>
       </c>
       <c r="AA125" s="41" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="AC125" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17711,10 +17767,10 @@
         <v>小·聒噪海贝</v>
       </c>
       <c r="AA126" s="41" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="AB126" s="5" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="AC126" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17744,10 +17800,10 @@
         <v>小·聒噪海贝</v>
       </c>
       <c r="AA127" s="41" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="AB127" s="5" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="AC127" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17777,7 +17833,7 @@
         <v>小·聒噪海贝</v>
       </c>
       <c r="AA128" s="41" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="AC128" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17799,7 +17855,7 @@
         <v>小·海藻小妖</v>
       </c>
       <c r="AA129" s="41" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="AC129" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17821,10 +17877,10 @@
         <v>小·海藻小妖</v>
       </c>
       <c r="AA130" s="41" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="AB130" s="5" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="AC130" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17846,7 +17902,7 @@
         <v>小·海藻小妖</v>
       </c>
       <c r="AA131" s="41" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="AC131" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17868,7 +17924,7 @@
         <v>小·海藻小妖</v>
       </c>
       <c r="AA132" s="41" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="AC132" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17890,10 +17946,10 @@
         <v>小·海藻小妖</v>
       </c>
       <c r="AA133" s="41" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="AB133" s="5" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="AC133" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17915,7 +17971,7 @@
         <v>小·海藻小妖</v>
       </c>
       <c r="AA134" s="41" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AC134" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17937,7 +17993,7 @@
         <v>小·海藻小妖</v>
       </c>
       <c r="AA135" s="41" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="AC135" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17998,58 +18054,58 @@
   <sheetData>
     <row r="1" ht="28.5" spans="1:30">
       <c r="A1" s="29" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="H1" s="29" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="I1" s="29" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="J1" s="29" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="K1" s="29" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="L1" s="29" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="M1" s="32" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="N1" s="32" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="O1" s="32" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="P1" s="32" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="Q1" s="32" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="R1" s="32" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="T1" s="33" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="V1" s="33" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
     </row>
     <row r="2" spans="1:30">
@@ -18262,14 +18318,14 @@
         <v/>
       </c>
       <c r="Z7" s="35" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="AA7" s="35"/>
       <c r="AB7" s="36">
         <v>10000</v>
       </c>
       <c r="AC7" s="37" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="AD7" s="37"/>
     </row>
@@ -18314,7 +18370,7 @@
         <v>10000=0.0048;600109=0.0001</v>
       </c>
       <c r="Z8" s="35" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="AA8" s="35"/>
       <c r="AB8" s="38">
@@ -18322,7 +18378,7 @@
         <v>0.0001</v>
       </c>
       <c r="AC8" s="37" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="AD8" s="37"/>
     </row>
@@ -18367,14 +18423,14 @@
         <v>10000=0.0048;600109=0.0001</v>
       </c>
       <c r="Z9" s="35" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="AA9" s="35"/>
       <c r="AB9" s="36">
         <v>300</v>
       </c>
       <c r="AC9" s="37" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="AD9" s="37"/>
     </row>
@@ -20927,7 +20983,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{f5b456f4-8295-4178-b25e-fd0bdce02cc2}</x14:id>
+          <x14:id>{c9fab3e9-a29d-4a79-9cc0-a65cc764b9f9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -20940,7 +20996,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{f5b456f4-8295-4178-b25e-fd0bdce02cc2}">
+          <x14:cfRule type="dataBar" id="{c9fab3e9-a29d-4a79-9cc0-a65cc764b9f9}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>-10</xm:f>
@@ -20994,17 +21050,17 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="D1" s="14"/>
       <c r="E1" s="6" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
@@ -21014,15 +21070,15 @@
       <c r="L1" s="15"/>
       <c r="M1" s="16"/>
       <c r="N1" s="6" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="P1" s="16"/>
       <c r="Q1" s="16"/>
       <c r="R1" s="6" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2" s="7" customFormat="1" spans="1:18">
@@ -21037,7 +21093,7 @@
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="7" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>32</v>
@@ -21053,7 +21109,7 @@
         <v>28</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="P2" s="16"/>
       <c r="Q2" s="16"/>
@@ -21063,58 +21119,58 @@
     </row>
     <row r="3" s="8" customFormat="1" ht="52.5" spans="1:18">
       <c r="A3" s="18" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="K3" s="21" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="L3" s="21" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="M3" s="22" t="s">
         <v>61</v>
       </c>
       <c r="N3" s="20" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="O3" s="20" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="P3" s="22" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="Q3" s="22" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -21144,7 +21200,7 @@
         <v>1311101</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="N4" s="23" t="str">
         <f>_xlfn.TEXTJOIN("_",1,"Car_AI",$M4)</f>
@@ -21191,7 +21247,7 @@
         <v>1311101</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="N5" s="23" t="str">
         <f t="shared" ref="N5:N13" si="0">_xlfn.TEXTJOIN("_",1,"Car_AI",$M5)</f>
@@ -21238,7 +21294,7 @@
         <v>1311101</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="N6" s="23" t="str">
         <f t="shared" si="0"/>
@@ -21285,7 +21341,7 @@
         <v>1311101</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="N7" s="23" t="str">
         <f t="shared" si="0"/>
@@ -21335,7 +21391,7 @@
         <v>1311101</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="N8" s="23" t="str">
         <f t="shared" si="0"/>
@@ -21385,7 +21441,7 @@
         <v>1311101</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="N9" s="23" t="str">
         <f t="shared" si="0"/>
@@ -21432,7 +21488,7 @@
         <v>1321101</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="N11" s="23" t="str">
         <f t="shared" si="0"/>
@@ -21479,7 +21535,7 @@
         <v>1321101</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="N12" s="23" t="str">
         <f t="shared" si="0"/>
@@ -21526,7 +21582,7 @@
         <v>1321101</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="N13" s="23" t="str">
         <f t="shared" si="0"/>
@@ -21579,7 +21635,7 @@
         <v>1311101</v>
       </c>
       <c r="M15" s="11" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="N15" s="23" t="str">
         <f t="shared" ref="N15:N21" si="2">_xlfn.TEXTJOIN("_",1,"Car_AI",$M15)</f>
@@ -21629,7 +21685,7 @@
         <v>1311102</v>
       </c>
       <c r="M16" s="11" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="N16" s="23" t="str">
         <f t="shared" si="2"/>
@@ -21682,7 +21738,7 @@
         <v>1311101</v>
       </c>
       <c r="M18" s="11" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="N18" s="23" t="str">
         <f t="shared" si="2"/>
@@ -21735,7 +21791,7 @@
         <v>1311102</v>
       </c>
       <c r="M19" s="11" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="N19" s="23" t="str">
         <f t="shared" si="2"/>
@@ -21788,7 +21844,7 @@
         <v>1311101</v>
       </c>
       <c r="M20" s="11" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="N20" s="23" t="str">
         <f t="shared" si="2"/>
@@ -21841,7 +21897,7 @@
         <v>1311102</v>
       </c>
       <c r="M21" s="11" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="N21" s="23" t="str">
         <f t="shared" si="2"/>
@@ -21872,7 +21928,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="E23" s="3">
         <v>101101</v>
@@ -21888,10 +21944,10 @@
         <v>1321101</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="N23" s="23" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="O23" s="3" t="str">
         <f t="shared" si="1"/>
@@ -21934,7 +21990,7 @@
         <v>1321101</v>
       </c>
       <c r="M25" s="11" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="N25" s="23" t="str">
         <f t="shared" ref="N25:N29" si="3">_xlfn.TEXTJOIN("_",1,"Car_AI",$M25)</f>
@@ -21984,7 +22040,7 @@
         <v>1321101</v>
       </c>
       <c r="M26" s="11" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="N26" s="23" t="str">
         <f t="shared" si="3"/>
@@ -22031,7 +22087,7 @@
         <v>1321101</v>
       </c>
       <c r="M28" s="11" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="N28" s="23" t="str">
         <f t="shared" si="3"/>
@@ -22081,7 +22137,7 @@
         <v>1321101</v>
       </c>
       <c r="M29" s="11" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="N29" s="23" t="str">
         <f t="shared" si="3"/>
@@ -22126,7 +22182,7 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" s="4" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -22138,7 +22194,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
     </row>
     <row r="4" spans="2:4">
@@ -22146,7 +22202,7 @@
         <v>10000</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="D4" s="3"/>
     </row>
@@ -22160,7 +22216,7 @@
         <v>600101</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="D6" s="3"/>
     </row>
@@ -22169,7 +22225,7 @@
         <v>600102</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="D7" s="3"/>
     </row>
@@ -22178,7 +22234,7 @@
         <v>600103</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="D8" s="3"/>
     </row>
@@ -22187,7 +22243,7 @@
         <v>600104</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="D9" s="3"/>
     </row>
@@ -22196,7 +22252,7 @@
         <v>600105</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="D10" s="3"/>
     </row>
@@ -22205,7 +22261,7 @@
         <v>600106</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="D11" s="3"/>
     </row>
@@ -22214,7 +22270,7 @@
         <v>600107</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="D12" s="3"/>
     </row>
@@ -22223,7 +22279,7 @@
         <v>600108</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="D13" s="3"/>
     </row>
@@ -22232,7 +22288,7 @@
         <v>600109</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="D14" s="3"/>
     </row>
@@ -22241,7 +22297,7 @@
         <v>600110</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="D15" s="3"/>
     </row>
@@ -22255,7 +22311,7 @@
         <v>600401</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="D17" s="3"/>
     </row>
@@ -22264,7 +22320,7 @@
         <v>600402</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="D18" s="3"/>
     </row>
@@ -22273,7 +22329,7 @@
         <v>600403</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="D19" s="3"/>
     </row>
@@ -22282,7 +22338,7 @@
         <v>600404</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="D20" s="3"/>
     </row>
@@ -22291,7 +22347,7 @@
         <v>600405</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="D21" s="3"/>
     </row>
@@ -22300,7 +22356,7 @@
         <v>600406</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="D22" s="3"/>
     </row>
@@ -22309,7 +22365,7 @@
         <v>600407</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="D23" s="3"/>
     </row>
@@ -22318,7 +22374,7 @@
         <v>600408</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="D24" s="3"/>
     </row>
@@ -22327,7 +22383,7 @@
         <v>600409</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="D25" s="3"/>
     </row>
@@ -22336,7 +22392,7 @@
         <v>600410</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="D26" s="3"/>
     </row>
@@ -22350,7 +22406,7 @@
         <v>600701</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="D28" s="3"/>
     </row>
@@ -22359,7 +22415,7 @@
         <v>600702</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="D29" s="3"/>
     </row>
@@ -22368,7 +22424,7 @@
         <v>600703</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="D30" s="3"/>
     </row>
@@ -22377,7 +22433,7 @@
         <v>600704</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="D31" s="3"/>
     </row>
@@ -22386,7 +22442,7 @@
         <v>600705</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="D32" s="3"/>
     </row>
@@ -22395,7 +22451,7 @@
         <v>600706</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="D33" s="3"/>
     </row>
@@ -22404,7 +22460,7 @@
         <v>600707</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="D34" s="3"/>
     </row>
@@ -22413,7 +22469,7 @@
         <v>600708</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="D35" s="3"/>
     </row>
@@ -22422,7 +22478,7 @@
         <v>600709</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="D36" s="3"/>
     </row>
@@ -22431,7 +22487,7 @@
         <v>600710</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="D37" s="3"/>
     </row>
@@ -22445,7 +22501,7 @@
         <v>600801</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="D39" s="3">
         <v>5</v>
@@ -22456,7 +22512,7 @@
         <v>600802</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="D40" s="3">
         <v>55</v>
@@ -22467,7 +22523,7 @@
         <v>600803</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="D41" s="3">
         <v>20</v>
@@ -22478,7 +22534,7 @@
         <v>600804</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="D42" s="3">
         <v>45</v>
@@ -22489,7 +22545,7 @@
         <v>600805</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="D43" s="3">
         <v>30</v>
@@ -22500,7 +22556,7 @@
         <v>600806</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="D44" s="3">
         <v>3</v>
@@ -22511,7 +22567,7 @@
         <v>600807</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="D45" s="3">
         <v>15</v>
@@ -22522,7 +22578,7 @@
         <v>600808</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="D46" s="3">
         <v>2</v>
@@ -22533,7 +22589,7 @@
         <v>600809</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="D47" s="3">
         <v>15</v>
@@ -22544,7 +22600,7 @@
         <v>600810</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="D48" s="3">
         <v>35</v>
@@ -22555,7 +22611,7 @@
         <v>600811</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="D49" s="3">
         <v>20</v>
@@ -22566,7 +22622,7 @@
         <v>600812</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="D50" s="3">
         <v>20</v>
@@ -22577,7 +22633,7 @@
         <v>600813</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="D51" s="3">
         <v>6</v>
@@ -22622,73 +22678,73 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="C7" s="2" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="C8" s="2" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="C9" s="2" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
     </row>
     <row r="11" spans="1:13">

</xml_diff>

<commit_message>
--Add 1309 1. 步行近战。
</commit_message>
<xml_diff>
--- a/Assets/Tables/table_enemy.xlsx
+++ b/Assets/Tables/table_enemy.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="470">
   <si>
     <t>id</t>
   </si>
@@ -1088,6 +1088,21 @@
   </si>
   <si>
     <t>JUMP_CD=0.58;ATTACK_DIS=5;JUMP_VELOCITY_X_MAX=20;JUMP_HEIGHT_AREA=1,2;BEFORE_ATTACK_SEC=0.6;AFTER_ATTACK_SEC=0.4;RUNNING_FIRE_COUNT=3</t>
+  </si>
+  <si>
+    <t>步行近战</t>
+  </si>
+  <si>
+    <t>sharp=4;blunt=4</t>
+  </si>
+  <si>
+    <t>monster_201815_Lake_Crab</t>
+  </si>
+  <si>
+    <t>BT_Lake_Crab</t>
+  </si>
+  <si>
+    <t>WALK_SPEED=4;ATK_DIS=0.5;BEFORE_ATTACK_SEC=0.27;AFTER_ATTACK_SEC=0.31;JUMP_HEIGHT_AREA=1,2</t>
   </si>
   <si>
     <t>parm_key</t>
@@ -3496,14 +3511,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AT86"/>
+  <dimension ref="A1:AT87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="AM61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="AN61" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AT86" sqref="AT86"/>
+      <selection pane="bottomRight" activeCell="AO87" sqref="AO87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
@@ -11118,7 +11133,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="86" spans="1:46">
+    <row r="86" ht="13" customHeight="1" spans="1:46">
       <c r="A86" s="24">
         <v>209104</v>
       </c>
@@ -11178,6 +11193,73 @@
       </c>
       <c r="AT86" t="s">
         <v>254</v>
+      </c>
+    </row>
+    <row r="87" spans="1:46">
+      <c r="A87" s="24">
+        <v>209105</v>
+      </c>
+      <c r="B87" s="24"/>
+      <c r="C87" s="25"/>
+      <c r="D87" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="G87" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H87" s="67">
+        <v>3000</v>
+      </c>
+      <c r="I87" s="24">
+        <v>0</v>
+      </c>
+      <c r="J87" s="24">
+        <v>7.25</v>
+      </c>
+      <c r="K87" s="24"/>
+      <c r="M87" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="N87" s="47">
+        <v>4</v>
+      </c>
+      <c r="O87" s="47">
+        <v>4</v>
+      </c>
+      <c r="AA87" t="s">
+        <v>257</v>
+      </c>
+      <c r="AB87" s="50"/>
+      <c r="AC87" t="s">
+        <v>258</v>
+      </c>
+      <c r="AE87" s="24">
+        <v>0.15</v>
+      </c>
+      <c r="AF87" s="24"/>
+      <c r="AG87" t="s">
+        <v>228</v>
+      </c>
+      <c r="AH87" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI87" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ87" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK87" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN87" s="24">
+        <v>0</v>
+      </c>
+      <c r="AO87" s="24" t="s">
+        <v>236</v>
+      </c>
+      <c r="AT87" t="s">
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -11241,19 +11323,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>0</v>
@@ -11262,19 +11344,19 @@
         <v>1</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="Q3" s="5" t="s">
         <v>0</v>
@@ -11283,19 +11365,19 @@
         <v>1</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="Y3" s="5" t="s">
         <v>0</v>
@@ -11304,19 +11386,19 @@
         <v>1</v>
       </c>
       <c r="AA3" s="5" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="AB3" s="5" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="AC3" s="5" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="AD3" s="5" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="AE3" s="5" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:42">
@@ -11335,10 +11417,10 @@
         <v>毒刺果实丛</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="M4" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11358,7 +11440,7 @@
         <v>涂涂鸟</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="U4" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11378,7 +11460,7 @@
         <v>金鱼</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="AC4" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11407,7 +11489,7 @@
         <v>毒刺果实丛</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="M5" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11427,7 +11509,7 @@
         <v>涂涂鸟</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="U5" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11447,10 +11529,10 @@
         <v>金鱼</v>
       </c>
       <c r="AA5" s="3" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="AB5" s="5" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="AC5" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11479,7 +11561,7 @@
         <v>毒刺果实丛</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="M6" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11499,7 +11581,7 @@
         <v>涂涂鸟</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="U6" s="92" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11519,7 +11601,7 @@
         <v>金鱼</v>
       </c>
       <c r="AA6" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AC6" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11532,16 +11614,16 @@
         <v>236</v>
       </c>
       <c r="AF6" s="29" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="AG6" s="29" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="AH6" s="29" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="AI6" s="29" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:42">
@@ -11560,7 +11642,7 @@
         <v>画中仙</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="M7" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11580,7 +11662,7 @@
         <v>涂涂鸟</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="U7" s="5" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11600,7 +11682,7 @@
         <v>金鱼</v>
       </c>
       <c r="AA7" s="3" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="AC7" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11662,7 +11744,7 @@
         <v>画中仙</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="M8" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11682,7 +11764,7 @@
         <v>涂涂鸟</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="U8" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11702,10 +11784,10 @@
         <v>金鱼</v>
       </c>
       <c r="AA8" s="3" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="AB8" s="5" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="AC8" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11721,7 +11803,7 @@
         <v>201402</v>
       </c>
       <c r="AG8" s="40" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="AH8" s="3">
         <f t="shared" ref="AH8:AH25" si="0">IFERROR(COLUMNS(_xlfn.TEXTSPLIT(AG8,";")),0)</f>
@@ -11768,7 +11850,7 @@
         <v>画中仙</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="M9" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11788,7 +11870,7 @@
         <v>涂涂鸟</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="U9" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11808,7 +11890,7 @@
         <v>金鱼</v>
       </c>
       <c r="AA9" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="AC9" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11869,7 +11951,7 @@
         <v>画中仙</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="M10" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11889,7 +11971,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="U10" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -11909,7 +11991,7 @@
         <v>金鱼</v>
       </c>
       <c r="AA10" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="AC10" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -11925,7 +12007,7 @@
         <v>201404</v>
       </c>
       <c r="AG10" s="40" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="AH10" s="3">
         <f t="shared" si="0"/>
@@ -11972,7 +12054,7 @@
         <v>画中仙</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="M11" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -11992,7 +12074,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="U11" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12012,10 +12094,10 @@
         <v>金鱼</v>
       </c>
       <c r="AA11" s="3" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="AB11" s="5" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="AC11" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12031,7 +12113,7 @@
         <v>201405</v>
       </c>
       <c r="AG11" s="40" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="AH11" s="3">
         <f t="shared" si="0"/>
@@ -12078,7 +12160,7 @@
         <v>画中仙</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="M12" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12098,7 +12180,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S12" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="U12" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12118,10 +12200,10 @@
         <v>金鱼</v>
       </c>
       <c r="AA12" s="3" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="AB12" s="5" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="AC12" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12137,7 +12219,7 @@
         <v>201406</v>
       </c>
       <c r="AG12" s="40" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="AH12" s="3">
         <f t="shared" si="0"/>
@@ -12177,7 +12259,7 @@
         <v>画中仙</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="M13" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12197,7 +12279,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S13" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="U13" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12217,7 +12299,7 @@
         <v>金鱼泡泡</v>
       </c>
       <c r="AA13" s="3" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="AC13" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12233,7 +12315,7 @@
         <v>201407</v>
       </c>
       <c r="AG13" s="40" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="AH13" s="3">
         <f t="shared" si="0"/>
@@ -12273,7 +12355,7 @@
         <v>画中仙</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="M14" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12293,7 +12375,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S14" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="U14" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12313,7 +12395,7 @@
         <v>金鱼泡泡</v>
       </c>
       <c r="AA14" s="3" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="AC14" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12367,7 +12449,7 @@
         <v>鱼妖</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="M15" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12387,7 +12469,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="U15" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12407,7 +12489,7 @@
         <v>海藻小妖</v>
       </c>
       <c r="AA15" s="3" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="AC15" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12461,7 +12543,7 @@
         <v>鱼妖</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="M16" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12481,7 +12563,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="U16" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12501,10 +12583,10 @@
         <v>海藻小妖</v>
       </c>
       <c r="AA16" s="3" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="AB16" s="5" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="AC16" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12558,10 +12640,10 @@
         <v>鬼瓮</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="M17" s="5" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12581,7 +12663,7 @@
         <v>沙漠蛇</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="U17" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12601,7 +12683,7 @@
         <v>海藻小妖</v>
       </c>
       <c r="AA17" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AC17" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12655,7 +12737,7 @@
         <v>鬼狰</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="M18" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12675,7 +12757,7 @@
         <v>巨牙蝎</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="U18" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12695,7 +12777,7 @@
         <v>海藻小妖</v>
       </c>
       <c r="AA18" s="3" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="AC18" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12749,7 +12831,7 @@
         <v>鬼狰</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="M19" s="5" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12769,7 +12851,7 @@
         <v>巨牙蝎</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="U19" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12789,10 +12871,10 @@
         <v>海藻小妖</v>
       </c>
       <c r="AA19" s="3" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="AB19" s="5" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="AC19" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12846,7 +12928,7 @@
         <v>鬼狰</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="M20" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_04[[#This Row],[v1]],tb_diy_04[[#This Row],[v2]])</f>
@@ -12866,7 +12948,7 @@
         <v>巨牙蝎</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="U20" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12886,7 +12968,7 @@
         <v>海藻小妖</v>
       </c>
       <c r="AA20" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="AC20" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -12941,10 +13023,10 @@
         <v>巨牙蝎</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="T21" s="5" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="U21" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -12964,7 +13046,7 @@
         <v>海藻小妖</v>
       </c>
       <c r="AA21" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="AC21" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13019,7 +13101,7 @@
         <v>巨牙蝎</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="U22" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13039,7 +13121,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA22" s="3" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="AC22" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13094,7 +13176,7 @@
         <v>巨牙蝎</v>
       </c>
       <c r="S23" s="3" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="U23" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13114,7 +13196,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA23" s="3" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="AC23" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13169,7 +13251,7 @@
         <v>巨牙蝎</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="U24" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13189,7 +13271,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA24" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AC24" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13244,7 +13326,7 @@
         <v>巨型石头人</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="U25" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13264,7 +13346,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA25" s="3" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="AC25" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13319,7 +13401,7 @@
         <v>巨型石头人</v>
       </c>
       <c r="S26" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="U26" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13339,7 +13421,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA26" s="3" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="AC26" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13362,7 +13444,7 @@
         <v>巨型石头人</v>
       </c>
       <c r="S27" s="3" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="U27" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13382,7 +13464,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA27" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="AC27" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13405,7 +13487,7 @@
         <v>巨型石头人</v>
       </c>
       <c r="S28" s="3" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="U28" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13425,7 +13507,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA28" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="AC28" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13448,7 +13530,7 @@
         <v>巨型石头人</v>
       </c>
       <c r="S29" s="3" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="U29" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13468,7 +13550,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA29" s="3" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="AC29" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13491,7 +13573,7 @@
         <v>小石头人</v>
       </c>
       <c r="S30" s="3" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="U30" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13511,7 +13593,7 @@
         <v>鲶鱼</v>
       </c>
       <c r="AA30" s="3" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="AC30" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13534,7 +13616,7 @@
         <v>小石头人</v>
       </c>
       <c r="S31" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="U31" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13554,7 +13636,7 @@
         <v>似目草</v>
       </c>
       <c r="AA31" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="AC31" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13577,7 +13659,7 @@
         <v>小石头人</v>
       </c>
       <c r="S32" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="U32" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13597,7 +13679,7 @@
         <v>似目草</v>
       </c>
       <c r="AA32" s="3" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="AC32" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13620,7 +13702,7 @@
         <v>小石头人</v>
       </c>
       <c r="S33" s="3" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="U33" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13640,7 +13722,7 @@
         <v>似目草</v>
       </c>
       <c r="AA33" s="5" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="AC33" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13666,7 +13748,7 @@
         <v>小石头人</v>
       </c>
       <c r="S34" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="U34" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13686,7 +13768,7 @@
         <v>脑型大水母</v>
       </c>
       <c r="AA34" s="3" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="AC34" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13708,7 +13790,7 @@
         <v>小石头人</v>
       </c>
       <c r="S35" s="3" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="T35" s="5"/>
       <c r="U35" s="3" t="str">
@@ -13729,7 +13811,7 @@
         <v>脑型大水母</v>
       </c>
       <c r="AA35" s="3" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="AC35" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13751,7 +13833,7 @@
         <v>小石头人</v>
       </c>
       <c r="S36" s="3" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="U36" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13771,7 +13853,7 @@
         <v>脑型大水母</v>
       </c>
       <c r="AA36" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AC36" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13793,10 +13875,10 @@
         <v>大盾守卫</v>
       </c>
       <c r="S37" s="3" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="T37" s="5" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="U37" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13816,7 +13898,7 @@
         <v>脑型大水母</v>
       </c>
       <c r="AA37" s="3" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="AC37" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13829,13 +13911,13 @@
         <v>236</v>
       </c>
       <c r="AF37" s="29" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="AG37" s="29" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="AH37" s="29" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
     </row>
     <row r="38" spans="10:35">
@@ -13847,10 +13929,10 @@
         <v>大盾守卫</v>
       </c>
       <c r="S38" s="3" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="T38" s="5" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="U38" s="5" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13870,7 +13952,7 @@
         <v>脑型大水母</v>
       </c>
       <c r="AA38" s="3" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="AC38" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13907,7 +13989,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S39" s="3" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="U39" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13927,10 +14009,10 @@
         <v>脑型大水母</v>
       </c>
       <c r="AA39" s="3" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="AB39" s="5" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="AC39" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -13966,7 +14048,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S40" s="3" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="U40" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -13986,7 +14068,7 @@
         <v>脑型大水母</v>
       </c>
       <c r="AA40" s="3" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="AC40" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14022,7 +14104,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S41" s="3" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="U41" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14042,7 +14124,7 @@
         <v>针刺小水母</v>
       </c>
       <c r="AA41" s="3" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="AC41" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14078,7 +14160,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S42" s="3" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="U42" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14098,7 +14180,7 @@
         <v>针刺小水母</v>
       </c>
       <c r="AA42" s="3" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="AC42" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14134,7 +14216,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S43" s="3" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="U43" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14154,7 +14236,7 @@
         <v>针刺小水母</v>
       </c>
       <c r="AA43" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AC43" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14190,7 +14272,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S44" s="3" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="U44" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14210,7 +14292,7 @@
         <v>针刺小水母</v>
       </c>
       <c r="AA44" s="3" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="AC44" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14246,7 +14328,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S45" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="U45" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14266,7 +14348,7 @@
         <v>针刺小水母</v>
       </c>
       <c r="AA45" s="3" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="AC45" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14302,7 +14384,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S46" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="U46" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14322,7 +14404,7 @@
         <v>针刺小水母</v>
       </c>
       <c r="AA46" s="3" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="AC46" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14358,7 +14440,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S47" s="3" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="U47" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14378,7 +14460,7 @@
         <v>印花水母</v>
       </c>
       <c r="AA47" s="3" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="AC47" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14414,7 +14496,7 @@
         <v>大盾守卫</v>
       </c>
       <c r="S48" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="U48" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14434,7 +14516,7 @@
         <v>印花水母</v>
       </c>
       <c r="AA48" s="3" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="AC48" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14470,10 +14552,10 @@
         <v>大盾守卫</v>
       </c>
       <c r="S49" s="3" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="T49" s="5" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="U49" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14493,7 +14575,7 @@
         <v>印花水母</v>
       </c>
       <c r="AA49" s="3" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="AC49" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14529,10 +14611,10 @@
         <v>基础守卫</v>
       </c>
       <c r="S50" s="3" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="T50" s="5" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="U50" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14552,7 +14634,7 @@
         <v>印花水母</v>
       </c>
       <c r="AA50" s="3" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="AC50" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14588,10 +14670,10 @@
         <v>基础守卫</v>
       </c>
       <c r="S51" s="3" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="T51" s="5" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="U51" s="5" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14611,7 +14693,7 @@
         <v>印花水母</v>
       </c>
       <c r="AA51" s="3" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="AC51" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14647,7 +14729,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S52" s="3" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="U52" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14667,7 +14749,7 @@
         <v>印花水母</v>
       </c>
       <c r="AA52" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="AC52" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14703,7 +14785,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S53" s="3" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="U53" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14723,7 +14805,7 @@
         <v>混沌沼泽怪</v>
       </c>
       <c r="AA53" s="3" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="AC53" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14759,10 +14841,10 @@
         <v>基础守卫</v>
       </c>
       <c r="S54" s="3" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="T54" s="5" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="U54" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14782,7 +14864,7 @@
         <v>混沌沼泽怪</v>
       </c>
       <c r="AA54" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="AC54" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14818,10 +14900,10 @@
         <v>基础守卫</v>
       </c>
       <c r="S55" s="3" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="T55" s="5" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="U55" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14841,7 +14923,7 @@
         <v>混沌沼泽怪</v>
       </c>
       <c r="AA55" s="3" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="AC55" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14871,7 +14953,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S56" s="3" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="U56" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14891,7 +14973,7 @@
         <v>混沌沼泽怪</v>
       </c>
       <c r="AA56" s="3" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="AC56" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14921,7 +15003,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S57" s="3" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="U57" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14941,7 +15023,7 @@
         <v>混沌沼泽怪</v>
       </c>
       <c r="AA57" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="AC57" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -14971,7 +15053,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S58" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="U58" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -14991,7 +15073,7 @@
         <v>混沌沼泽怪</v>
       </c>
       <c r="AA58" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="AC58" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15021,7 +15103,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S59" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="U59" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15041,7 +15123,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA59" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="AC59" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15071,7 +15153,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S60" s="3" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="U60" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15091,7 +15173,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA60" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="AC60" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15121,7 +15203,7 @@
         <v>基础守卫</v>
       </c>
       <c r="S61" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="U61" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15141,7 +15223,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA61" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="AC61" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15171,10 +15253,10 @@
         <v>基础守卫</v>
       </c>
       <c r="S62" s="3" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="T62" s="5" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="U62" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15194,7 +15276,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA62" s="3" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="AC62" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15224,7 +15306,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S63" s="3" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="U63" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15244,7 +15326,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA63" s="3" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="AC63" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15274,7 +15356,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S64" s="3" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="U64" s="5" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15294,7 +15376,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA64" s="3" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="AC64" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15324,7 +15406,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S65" s="3" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="U65" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15344,7 +15426,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA65" s="3" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="AC65" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15374,7 +15456,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S66" s="3" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="U66" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15394,7 +15476,7 @@
         <v>青蛙</v>
       </c>
       <c r="AA66" s="3" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="AC66" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15424,7 +15506,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S67" s="3" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="U67" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15444,7 +15526,7 @@
         <v/>
       </c>
       <c r="AA67" s="3" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="AC67" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15474,7 +15556,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S68" s="3" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="U68" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15494,10 +15576,10 @@
         <v/>
       </c>
       <c r="AA68" s="3" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="AB68" s="5" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="AC68" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15527,7 +15609,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S69" s="3" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="U69" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15547,10 +15629,10 @@
         <v/>
       </c>
       <c r="AA69" s="3" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="AB69" s="5" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="AC69" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15580,7 +15662,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S70" s="3" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="U70" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15600,7 +15682,7 @@
         <v/>
       </c>
       <c r="AA70" s="3" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="AC70" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15630,7 +15712,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S71" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="U71" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15650,7 +15732,7 @@
         <v>贝壳乌贼</v>
       </c>
       <c r="AA71" s="3" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="AC71" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15680,7 +15762,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S72" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="U72" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15700,7 +15782,7 @@
         <v>贝壳乌贼</v>
       </c>
       <c r="AA72" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="AC72" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15730,7 +15812,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S73" s="3" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="U73" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15750,7 +15832,7 @@
         <v>贝壳乌贼</v>
       </c>
       <c r="AA73" s="3" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="AC73" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15780,7 +15862,7 @@
         <v>双刀守卫</v>
       </c>
       <c r="S74" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="U74" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15800,7 +15882,7 @@
         <v>贝壳乌贼</v>
       </c>
       <c r="AA74" s="3" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="AC74" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15830,10 +15912,10 @@
         <v>双刀守卫</v>
       </c>
       <c r="S75" s="3" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="T75" s="5" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="U75" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15853,7 +15935,7 @@
         <v>贝壳乌贼</v>
       </c>
       <c r="AA75" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="AC75" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15883,7 +15965,7 @@
         <v>大仙人掌</v>
       </c>
       <c r="S76" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="U76" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15903,7 +15985,7 @@
         <v>贝壳乌贼</v>
       </c>
       <c r="AA76" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="AC76" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15933,7 +16015,7 @@
         <v>大仙人掌</v>
       </c>
       <c r="S77" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="U77" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -15953,7 +16035,7 @@
         <v>弱小螃蟹</v>
       </c>
       <c r="AA77" s="3" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="AC77" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -15983,10 +16065,10 @@
         <v>大仙人掌</v>
       </c>
       <c r="S78" s="3" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="T78" s="5" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="U78" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16006,7 +16088,7 @@
         <v>弱小螃蟹</v>
       </c>
       <c r="AA78" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="AC78" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16036,10 +16118,10 @@
         <v>大仙人掌</v>
       </c>
       <c r="S79" s="3" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="T79" s="5" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="U79" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16059,7 +16141,7 @@
         <v>弱小螃蟹</v>
       </c>
       <c r="AA79" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="AC79" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16089,7 +16171,7 @@
         <v>小仙人掌</v>
       </c>
       <c r="S80" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="U80" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16109,7 +16191,7 @@
         <v>弱小螃蟹</v>
       </c>
       <c r="AA80" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="AC80" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16139,7 +16221,7 @@
         <v>小仙人掌</v>
       </c>
       <c r="S81" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="U81" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16159,7 +16241,7 @@
         <v>大钳螃蟹</v>
       </c>
       <c r="AA81" s="3" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="AC81" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16189,10 +16271,10 @@
         <v>小仙人掌</v>
       </c>
       <c r="S82" s="3" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="T82" s="5" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="U82" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16212,7 +16294,7 @@
         <v>大钳螃蟹</v>
       </c>
       <c r="AA82" s="3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="AC82" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16242,10 +16324,10 @@
         <v>小仙人掌</v>
       </c>
       <c r="S83" s="3" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="T83" s="5" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="U83" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16265,7 +16347,7 @@
         <v>大钳螃蟹</v>
       </c>
       <c r="AA83" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="AC83" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16295,7 +16377,7 @@
         <v>大风滚草</v>
       </c>
       <c r="S84" s="3" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="U84" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16315,7 +16397,7 @@
         <v>大钳螃蟹</v>
       </c>
       <c r="AA84" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="AC84" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16345,7 +16427,7 @@
         <v>大风滚草</v>
       </c>
       <c r="S85" s="3" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="U85" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16365,7 +16447,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA85" s="3" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="AC85" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16395,7 +16477,7 @@
         <v>大风滚草</v>
       </c>
       <c r="S86" s="3" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="U86" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16415,7 +16497,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA86" s="3" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="AC86" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16445,7 +16527,7 @@
         <v>大风滚草</v>
       </c>
       <c r="S87" s="3" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="U87" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16465,7 +16547,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA87" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AC87" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16495,7 +16577,7 @@
         <v>大风滚草</v>
       </c>
       <c r="S88" s="3" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="U88" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16515,7 +16597,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA88" s="3" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="AC88" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16545,7 +16627,7 @@
         <v>小风滚草</v>
       </c>
       <c r="S89" s="3" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="U89" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16565,7 +16647,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA89" s="3" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="AC89" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16595,7 +16677,7 @@
         <v>小风滚草</v>
       </c>
       <c r="S90" s="3" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="U90" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16615,7 +16697,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA90" s="3" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="AC90" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16645,7 +16727,7 @@
         <v>小风滚草</v>
       </c>
       <c r="S91" s="3" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="U91" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16665,7 +16747,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA91" s="3" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="AC91" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16695,7 +16777,7 @@
         <v>小风滚草</v>
       </c>
       <c r="S92" s="3" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="U92" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16715,7 +16797,7 @@
         <v>金鱼王</v>
       </c>
       <c r="AA92" s="3" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="AC92" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16745,7 +16827,7 @@
         <v>小风滚草</v>
       </c>
       <c r="S93" s="3" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="U93" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_07[[#This Row],[v1]],tb_diy_07[[#This Row],[v2]])</f>
@@ -16765,7 +16847,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA93" s="3" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="AC93" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16795,7 +16877,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA94" s="3" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="AC94" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16825,7 +16907,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA95" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AC95" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16855,7 +16937,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA96" s="3" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="AC96" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16885,7 +16967,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA97" s="3" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="AC97" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16915,7 +16997,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA98" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="AC98" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16945,7 +17027,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA99" s="3" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="AC99" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -16975,7 +17057,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA100" s="3" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="AC100" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17005,7 +17087,7 @@
         <v>渊齿</v>
       </c>
       <c r="AA101" s="3" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="AC101" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17035,7 +17117,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA102" s="3" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="AC102" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17065,7 +17147,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA103" s="3" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="AC103" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17095,7 +17177,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA104" s="3" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AC104" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17125,7 +17207,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA105" s="3" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="AC105" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17155,7 +17237,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA106" s="3" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="AC106" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17185,7 +17267,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA107" s="3" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="AC107" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17215,7 +17297,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA108" s="3" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="AC108" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17245,7 +17327,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA109" s="3" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="AC109" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17275,7 +17357,7 @@
         <v>缠绕水藻</v>
       </c>
       <c r="AA110" s="3" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="AC110" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17305,7 +17387,7 @@
         <v>聒噪海贝</v>
       </c>
       <c r="AA111" s="3" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="AC111" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17335,10 +17417,10 @@
         <v>聒噪海贝</v>
       </c>
       <c r="AA112" s="3" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="AB112" s="5" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="AC112" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17368,10 +17450,10 @@
         <v>聒噪海贝</v>
       </c>
       <c r="AA113" s="3" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="AB113" s="5" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="AC113" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17401,7 +17483,7 @@
         <v>聒噪海贝</v>
       </c>
       <c r="AA114" s="3" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="AC114" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17431,7 +17513,7 @@
         <v>凶猛海贝</v>
       </c>
       <c r="AA115" s="3" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="AC115" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17461,10 +17543,10 @@
         <v>凶猛海贝</v>
       </c>
       <c r="AA116" s="3" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="AB116" s="5" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="AC116" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17494,10 +17576,10 @@
         <v>凶猛海贝</v>
       </c>
       <c r="AA117" s="3" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="AB117" s="5" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="AC117" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17527,7 +17609,7 @@
         <v>凶猛海贝</v>
       </c>
       <c r="AA118" s="3" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="AC118" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17557,7 +17639,7 @@
         <v>小·印花水母</v>
       </c>
       <c r="AA119" s="41" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="AC119" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17587,7 +17669,7 @@
         <v>小·印花水母</v>
       </c>
       <c r="AA120" s="41" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="AC120" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17617,7 +17699,7 @@
         <v>小·印花水母</v>
       </c>
       <c r="AA121" s="41" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="AC121" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17647,7 +17729,7 @@
         <v>小·印花水母</v>
       </c>
       <c r="AA122" s="41" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="AC122" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17677,7 +17759,7 @@
         <v>小·印花水母</v>
       </c>
       <c r="AA123" s="41" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="AC123" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17707,7 +17789,7 @@
         <v>小·印花水母</v>
       </c>
       <c r="AA124" s="41" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="AC124" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17737,7 +17819,7 @@
         <v>小·聒噪海贝</v>
       </c>
       <c r="AA125" s="41" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="AC125" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17767,10 +17849,10 @@
         <v>小·聒噪海贝</v>
       </c>
       <c r="AA126" s="41" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="AB126" s="5" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="AC126" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17800,10 +17882,10 @@
         <v>小·聒噪海贝</v>
       </c>
       <c r="AA127" s="41" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="AB127" s="5" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="AC127" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17833,7 +17915,7 @@
         <v>小·聒噪海贝</v>
       </c>
       <c r="AA128" s="41" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="AC128" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17855,7 +17937,7 @@
         <v>小·海藻小妖</v>
       </c>
       <c r="AA129" s="41" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="AC129" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17877,10 +17959,10 @@
         <v>小·海藻小妖</v>
       </c>
       <c r="AA130" s="41" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="AB130" s="5" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="AC130" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17902,7 +17984,7 @@
         <v>小·海藻小妖</v>
       </c>
       <c r="AA131" s="41" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AC131" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17924,7 +18006,7 @@
         <v>小·海藻小妖</v>
       </c>
       <c r="AA132" s="41" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="AC132" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17946,10 +18028,10 @@
         <v>小·海藻小妖</v>
       </c>
       <c r="AA133" s="41" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="AB133" s="5" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="AC133" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17971,7 +18053,7 @@
         <v>小·海藻小妖</v>
       </c>
       <c r="AA134" s="41" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="AC134" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -17993,7 +18075,7 @@
         <v>小·海藻小妖</v>
       </c>
       <c r="AA135" s="41" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="AC135" s="41" t="str">
         <f>_xlfn.TEXTJOIN(",",1,tb_diy_08[[#This Row],[v1]],tb_diy_08[[#This Row],[v2]])</f>
@@ -18054,58 +18136,58 @@
   <sheetData>
     <row r="1" ht="28.5" spans="1:30">
       <c r="A1" s="29" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="H1" s="29" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="I1" s="29" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="J1" s="29" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
       <c r="K1" s="29" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="L1" s="29" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="M1" s="32" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="N1" s="32" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
       <c r="O1" s="32" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="P1" s="32" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
       <c r="Q1" s="32" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="R1" s="32" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="T1" s="33" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="V1" s="33" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
     </row>
     <row r="2" spans="1:30">
@@ -18318,14 +18400,14 @@
         <v/>
       </c>
       <c r="Z7" s="35" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="AA7" s="35"/>
       <c r="AB7" s="36">
         <v>10000</v>
       </c>
       <c r="AC7" s="37" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="AD7" s="37"/>
     </row>
@@ -18370,7 +18452,7 @@
         <v>10000=0.0048;600109=0.0001</v>
       </c>
       <c r="Z8" s="35" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="AA8" s="35"/>
       <c r="AB8" s="38">
@@ -18378,7 +18460,7 @@
         <v>0.0001</v>
       </c>
       <c r="AC8" s="37" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="AD8" s="37"/>
     </row>
@@ -18423,14 +18505,14 @@
         <v>10000=0.0048;600109=0.0001</v>
       </c>
       <c r="Z9" s="35" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="AA9" s="35"/>
       <c r="AB9" s="36">
         <v>300</v>
       </c>
       <c r="AC9" s="37" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="AD9" s="37"/>
     </row>
@@ -20983,7 +21065,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{a67b2a63-272f-4794-9389-9863d596408b}</x14:id>
+          <x14:id>{eba17967-7050-457c-8c41-8bc72cad80ee}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -20996,7 +21078,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{a67b2a63-272f-4794-9389-9863d596408b}">
+          <x14:cfRule type="dataBar" id="{eba17967-7050-457c-8c41-8bc72cad80ee}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>-10</xm:f>
@@ -21050,17 +21132,17 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="D1" s="14"/>
       <c r="E1" s="6" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
@@ -21070,15 +21152,15 @@
       <c r="L1" s="15"/>
       <c r="M1" s="16"/>
       <c r="N1" s="6" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="P1" s="16"/>
       <c r="Q1" s="16"/>
       <c r="R1" s="6" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
     </row>
     <row r="2" s="7" customFormat="1" spans="1:18">
@@ -21093,7 +21175,7 @@
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="7" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>32</v>
@@ -21109,7 +21191,7 @@
         <v>28</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="P2" s="16"/>
       <c r="Q2" s="16"/>
@@ -21119,58 +21201,58 @@
     </row>
     <row r="3" s="8" customFormat="1" ht="52.5" spans="1:18">
       <c r="A3" s="18" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="K3" s="21" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="L3" s="21" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="M3" s="22" t="s">
         <v>61</v>
       </c>
       <c r="N3" s="20" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="O3" s="20" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="P3" s="22" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="Q3" s="22" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -21200,7 +21282,7 @@
         <v>1311101</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="N4" s="23" t="str">
         <f>_xlfn.TEXTJOIN("_",1,"Car_AI",$M4)</f>
@@ -21247,7 +21329,7 @@
         <v>1311101</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="N5" s="23" t="str">
         <f t="shared" ref="N5:N13" si="0">_xlfn.TEXTJOIN("_",1,"Car_AI",$M5)</f>
@@ -21294,7 +21376,7 @@
         <v>1311101</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="N6" s="23" t="str">
         <f t="shared" si="0"/>
@@ -21341,7 +21423,7 @@
         <v>1311101</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="N7" s="23" t="str">
         <f t="shared" si="0"/>
@@ -21391,7 +21473,7 @@
         <v>1311101</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="N8" s="23" t="str">
         <f t="shared" si="0"/>
@@ -21441,7 +21523,7 @@
         <v>1311101</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="N9" s="23" t="str">
         <f t="shared" si="0"/>
@@ -21488,7 +21570,7 @@
         <v>1321101</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="N11" s="23" t="str">
         <f t="shared" si="0"/>
@@ -21535,7 +21617,7 @@
         <v>1321101</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="N12" s="23" t="str">
         <f t="shared" si="0"/>
@@ -21582,7 +21664,7 @@
         <v>1321101</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="N13" s="23" t="str">
         <f t="shared" si="0"/>
@@ -21635,7 +21717,7 @@
         <v>1311101</v>
       </c>
       <c r="M15" s="11" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="N15" s="23" t="str">
         <f t="shared" ref="N15:N21" si="2">_xlfn.TEXTJOIN("_",1,"Car_AI",$M15)</f>
@@ -21685,7 +21767,7 @@
         <v>1311102</v>
       </c>
       <c r="M16" s="11" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="N16" s="23" t="str">
         <f t="shared" si="2"/>
@@ -21738,7 +21820,7 @@
         <v>1311101</v>
       </c>
       <c r="M18" s="11" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="N18" s="23" t="str">
         <f t="shared" si="2"/>
@@ -21791,7 +21873,7 @@
         <v>1311102</v>
       </c>
       <c r="M19" s="11" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="N19" s="23" t="str">
         <f t="shared" si="2"/>
@@ -21844,7 +21926,7 @@
         <v>1311101</v>
       </c>
       <c r="M20" s="11" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="N20" s="23" t="str">
         <f t="shared" si="2"/>
@@ -21897,7 +21979,7 @@
         <v>1311102</v>
       </c>
       <c r="M21" s="11" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="N21" s="23" t="str">
         <f t="shared" si="2"/>
@@ -21928,7 +22010,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="E23" s="3">
         <v>101101</v>
@@ -21944,10 +22026,10 @@
         <v>1321101</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="N23" s="23" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="O23" s="3" t="str">
         <f t="shared" si="1"/>
@@ -21990,7 +22072,7 @@
         <v>1321101</v>
       </c>
       <c r="M25" s="11" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="N25" s="23" t="str">
         <f t="shared" ref="N25:N29" si="3">_xlfn.TEXTJOIN("_",1,"Car_AI",$M25)</f>
@@ -22040,7 +22122,7 @@
         <v>1321101</v>
       </c>
       <c r="M26" s="11" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="N26" s="23" t="str">
         <f t="shared" si="3"/>
@@ -22087,7 +22169,7 @@
         <v>1321101</v>
       </c>
       <c r="M28" s="11" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="N28" s="23" t="str">
         <f t="shared" si="3"/>
@@ -22137,7 +22219,7 @@
         <v>1321101</v>
       </c>
       <c r="M29" s="11" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="N29" s="23" t="str">
         <f t="shared" si="3"/>
@@ -22182,7 +22264,7 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" s="4" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -22194,7 +22276,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4" spans="2:4">
@@ -22202,7 +22284,7 @@
         <v>10000</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="D4" s="3"/>
     </row>
@@ -22216,7 +22298,7 @@
         <v>600101</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="D6" s="3"/>
     </row>
@@ -22225,7 +22307,7 @@
         <v>600102</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="D7" s="3"/>
     </row>
@@ -22234,7 +22316,7 @@
         <v>600103</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="D8" s="3"/>
     </row>
@@ -22243,7 +22325,7 @@
         <v>600104</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="D9" s="3"/>
     </row>
@@ -22252,7 +22334,7 @@
         <v>600105</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="D10" s="3"/>
     </row>
@@ -22261,7 +22343,7 @@
         <v>600106</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="D11" s="3"/>
     </row>
@@ -22270,7 +22352,7 @@
         <v>600107</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="D12" s="3"/>
     </row>
@@ -22279,7 +22361,7 @@
         <v>600108</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="D13" s="3"/>
     </row>
@@ -22288,7 +22370,7 @@
         <v>600109</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="D14" s="3"/>
     </row>
@@ -22297,7 +22379,7 @@
         <v>600110</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D15" s="3"/>
     </row>
@@ -22311,7 +22393,7 @@
         <v>600401</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="D17" s="3"/>
     </row>
@@ -22320,7 +22402,7 @@
         <v>600402</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="D18" s="3"/>
     </row>
@@ -22329,7 +22411,7 @@
         <v>600403</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="D19" s="3"/>
     </row>
@@ -22338,7 +22420,7 @@
         <v>600404</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="D20" s="3"/>
     </row>
@@ -22347,7 +22429,7 @@
         <v>600405</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="D21" s="3"/>
     </row>
@@ -22356,7 +22438,7 @@
         <v>600406</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="D22" s="3"/>
     </row>
@@ -22365,7 +22447,7 @@
         <v>600407</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="D23" s="3"/>
     </row>
@@ -22374,7 +22456,7 @@
         <v>600408</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="D24" s="3"/>
     </row>
@@ -22383,7 +22465,7 @@
         <v>600409</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c r="D25" s="3"/>
     </row>
@@ -22392,7 +22474,7 @@
         <v>600410</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c r="D26" s="3"/>
     </row>
@@ -22406,7 +22488,7 @@
         <v>600701</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c r="D28" s="3"/>
     </row>
@@ -22415,7 +22497,7 @@
         <v>600702</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="D29" s="3"/>
     </row>
@@ -22424,7 +22506,7 @@
         <v>600703</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
       <c r="D30" s="3"/>
     </row>
@@ -22433,7 +22515,7 @@
         <v>600704</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>428</v>
+        <v>433</v>
       </c>
       <c r="D31" s="3"/>
     </row>
@@ -22442,7 +22524,7 @@
         <v>600705</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="D32" s="3"/>
     </row>
@@ -22451,7 +22533,7 @@
         <v>600706</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="D33" s="3"/>
     </row>
@@ -22460,7 +22542,7 @@
         <v>600707</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
       <c r="D34" s="3"/>
     </row>
@@ -22469,7 +22551,7 @@
         <v>600708</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="D35" s="3"/>
     </row>
@@ -22478,7 +22560,7 @@
         <v>600709</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="D36" s="3"/>
     </row>
@@ -22487,7 +22569,7 @@
         <v>600710</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="D37" s="3"/>
     </row>
@@ -22501,7 +22583,7 @@
         <v>600801</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
       <c r="D39" s="3">
         <v>5</v>
@@ -22512,7 +22594,7 @@
         <v>600802</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="D40" s="3">
         <v>55</v>
@@ -22523,7 +22605,7 @@
         <v>600803</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="D41" s="3">
         <v>20</v>
@@ -22534,7 +22616,7 @@
         <v>600804</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="D42" s="3">
         <v>45</v>
@@ -22545,7 +22627,7 @@
         <v>600805</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="D43" s="3">
         <v>30</v>
@@ -22556,7 +22638,7 @@
         <v>600806</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="D44" s="3">
         <v>3</v>
@@ -22567,7 +22649,7 @@
         <v>600807</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c r="D45" s="3">
         <v>15</v>
@@ -22578,7 +22660,7 @@
         <v>600808</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="D46" s="3">
         <v>2</v>
@@ -22589,7 +22671,7 @@
         <v>600809</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="D47" s="3">
         <v>15</v>
@@ -22600,7 +22682,7 @@
         <v>600810</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="D48" s="3">
         <v>35</v>
@@ -22611,7 +22693,7 @@
         <v>600811</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="D49" s="3">
         <v>20</v>
@@ -22622,7 +22704,7 @@
         <v>600812</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>446</v>
+        <v>451</v>
       </c>
       <c r="D50" s="3">
         <v>20</v>
@@ -22633,7 +22715,7 @@
         <v>600813</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
       <c r="D51" s="3">
         <v>6</v>
@@ -22678,73 +22760,73 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="C7" s="2" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="C8" s="2" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="C9" s="2" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
     </row>
     <row r="11" spans="1:13">

</xml_diff>